<commit_message>
Revise the Lebanese Civil War
-Taif Agreement
-May 17 Agreement
-UNSC Resolution 1559
-Superstate Central Bank Interest rates and Common Market Tariffs do not apply to superstate countries
-Transport is enabled in 1946
-Climate Change protest event to raise progressive support among primarily the middle class starting from 2011
-Localisation tweaks
</commit_message>
<xml_diff>
--- a/Goods Production Calculator.xlsx
+++ b/Goods Production Calculator.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="146">
   <si>
     <t>small_arms</t>
   </si>
@@ -927,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CG148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BV43" workbookViewId="0">
-      <selection activeCell="CE69" sqref="CE69"/>
+    <sheetView tabSelected="1" topLeftCell="BI93" workbookViewId="0">
+      <selection activeCell="BQ108" sqref="BQ108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2946,11 +2946,11 @@
         <v>57</v>
       </c>
       <c r="CF20" s="10">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="CG20" s="11">
         <f>(CD24/CD25)-1</f>
-        <v>0.27049180327868849</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="1:85">
@@ -3159,9 +3159,16 @@
       <c r="BX22" s="10"/>
       <c r="BY22" s="10"/>
       <c r="BZ22" s="5"/>
-      <c r="CB22" s="3"/>
-      <c r="CC22" s="9"/>
-      <c r="CD22" s="9"/>
+      <c r="CB22" s="3">
+        <f t="shared" ref="CB22:CB23" si="4">VLOOKUP(CC22,$A:$B,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="CC22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="CD22" s="9">
+        <v>1</v>
+      </c>
       <c r="CE22" s="10"/>
       <c r="CF22" s="10"/>
       <c r="CG22" s="5"/>
@@ -3241,9 +3248,16 @@
       <c r="BX23" s="10"/>
       <c r="BY23" s="10"/>
       <c r="BZ23" s="5"/>
-      <c r="CB23" s="3"/>
-      <c r="CC23" s="9"/>
-      <c r="CD23" s="9"/>
+      <c r="CB23" s="3">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="CC23" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="CD23" s="9">
+        <v>1</v>
+      </c>
       <c r="CE23" s="10"/>
       <c r="CF23" s="10"/>
       <c r="CG23" s="5"/>
@@ -3385,7 +3399,7 @@
       </c>
       <c r="CD24" s="3">
         <f>SUM(CF20*CB24,CF21*CB25,CF22*CB26,CF23*CB27)</f>
-        <v>12.4</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="CG24" s="5"/>
     </row>
@@ -3493,7 +3507,7 @@
       </c>
       <c r="CD25" s="3">
         <f>SUM(CD20*CB20,CD21*CB21,CD22*CB22,CD23*CB23,CC27)</f>
-        <v>9.76</v>
+        <v>29.76</v>
       </c>
       <c r="CG25" s="5"/>
     </row>
@@ -4110,7 +4124,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="J32" s="3">
-        <f t="shared" ref="J32:J33" si="4">VLOOKUP(K32,$A:$B,2,FALSE)</f>
+        <f t="shared" ref="J32:J33" si="5">VLOOKUP(K32,$A:$B,2,FALSE)</f>
         <v>1.5</v>
       </c>
       <c r="K32" s="9" t="s">
@@ -4220,7 +4234,7 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="J33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6</v>
       </c>
       <c r="K33" s="9" t="s">
@@ -5197,7 +5211,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="J43" s="3">
-        <f t="shared" ref="J43:J44" si="5">VLOOKUP(K43,$A:$B,2,FALSE)</f>
+        <f t="shared" ref="J43:J44" si="6">VLOOKUP(K43,$A:$B,2,FALSE)</f>
         <v>1.5</v>
       </c>
       <c r="K43" s="9" t="s">
@@ -5308,7 +5322,7 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="J44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.6</v>
       </c>
       <c r="K44" s="9" t="s">
@@ -6120,7 +6134,7 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="J54" s="3">
-        <f t="shared" ref="J54:J55" si="6">VLOOKUP(K54,$A:$B,2,FALSE)</f>
+        <f t="shared" ref="J54:J55" si="7">VLOOKUP(K54,$A:$B,2,FALSE)</f>
         <v>1.5</v>
       </c>
       <c r="K54" s="9" t="s">
@@ -6207,7 +6221,7 @@
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="J55" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.6</v>
       </c>
       <c r="K55" s="9" t="s">
@@ -6757,7 +6771,7 @@
     </row>
     <row r="65" spans="10:85">
       <c r="J65" s="3">
-        <f t="shared" ref="J65:J66" si="7">VLOOKUP(K65,$A:$B,2,FALSE)</f>
+        <f t="shared" ref="J65:J66" si="8">VLOOKUP(K65,$A:$B,2,FALSE)</f>
         <v>1.5</v>
       </c>
       <c r="K65" s="9" t="s">
@@ -6810,7 +6824,7 @@
     </row>
     <row r="66" spans="10:85">
       <c r="J66" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.6</v>
       </c>
       <c r="K66" s="9" t="s">
@@ -6828,7 +6842,7 @@
       <c r="AB66" s="10"/>
       <c r="AC66" s="5"/>
       <c r="BN66" s="3">
-        <f t="shared" ref="BN66:BN67" si="8">VLOOKUP(BO66,$A:$B,2,FALSE)</f>
+        <f t="shared" ref="BN66:BN67" si="9">VLOOKUP(BO66,$A:$B,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="BO66" s="9" t="s">
@@ -6867,7 +6881,7 @@
       <c r="AB67" s="10"/>
       <c r="AC67" s="5"/>
       <c r="BN67" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.2</v>
       </c>
       <c r="BO67" s="9" t="s">
@@ -7155,7 +7169,7 @@
     </row>
     <row r="76" spans="10:85">
       <c r="J76" s="3">
-        <f t="shared" ref="J76:J77" si="9">VLOOKUP(K76,$A:$B,2,FALSE)</f>
+        <f t="shared" ref="J76:J77" si="10">VLOOKUP(K76,$A:$B,2,FALSE)</f>
         <v>1.5</v>
       </c>
       <c r="K76" s="9" t="s">
@@ -7195,7 +7209,7 @@
     </row>
     <row r="77" spans="10:85">
       <c r="J77" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6</v>
       </c>
       <c r="K77" s="9" t="s">
@@ -7736,7 +7750,7 @@
       <c r="AB99" s="10"/>
       <c r="AC99" s="5"/>
       <c r="BN99" s="3">
-        <f t="shared" ref="BN99:BN100" si="10">VLOOKUP(BO99,$A:$B,2,FALSE)</f>
+        <f t="shared" ref="BN99:BN100" si="11">VLOOKUP(BO99,$A:$B,2,FALSE)</f>
         <v>4.0999999999999996</v>
       </c>
       <c r="BO99" s="9" t="s">
@@ -7757,7 +7771,7 @@
       <c r="AB100" s="10"/>
       <c r="AC100" s="5"/>
       <c r="BN100" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="BO100" s="9" t="s">
@@ -7885,17 +7899,24 @@
         <v>49</v>
       </c>
       <c r="BR108" s="10">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="BS108" s="11">
         <f>(BP112/BP113)-1</f>
-        <v>0.2352610892756879</v>
+        <v>0.22386537480877111</v>
       </c>
     </row>
     <row r="109" spans="24:71">
-      <c r="BN109" s="3"/>
-      <c r="BO109" s="9"/>
-      <c r="BP109" s="9"/>
+      <c r="BN109" s="3">
+        <f>VLOOKUP(BO109,$A:$B,2,FALSE)</f>
+        <v>1.8</v>
+      </c>
+      <c r="BO109" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="BP109" s="9">
+        <v>1</v>
+      </c>
       <c r="BQ109" s="10"/>
       <c r="BR109" s="10"/>
       <c r="BS109" s="5"/>
@@ -7926,7 +7947,7 @@
       </c>
       <c r="BP112" s="3">
         <f>SUM(BR108*BN112,BR109*BN113,BR110*BN114,BR111*BN115)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="BS112" s="5"/>
     </row>
@@ -7937,7 +7958,7 @@
       </c>
       <c r="BP113" s="3">
         <f>SUM(BP108*BN108,BP109*BN109,BP110*BN110,BP111*BN111,BO115)</f>
-        <v>17.809999999999999</v>
+        <v>19.61</v>
       </c>
       <c r="BS113" s="5"/>
     </row>
@@ -8007,7 +8028,7 @@
     </row>
     <row r="120" spans="66:71">
       <c r="BN120" s="3">
-        <f t="shared" ref="BN120:BN122" si="11">VLOOKUP(BO120,$A:$B,2,FALSE)</f>
+        <f t="shared" ref="BN120:BN122" si="12">VLOOKUP(BO120,$A:$B,2,FALSE)</f>
         <v>1.8</v>
       </c>
       <c r="BO120" s="9" t="s">
@@ -8022,7 +8043,7 @@
     </row>
     <row r="121" spans="66:71">
       <c r="BN121" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.2</v>
       </c>
       <c r="BO121" s="9" t="s">
@@ -8037,7 +8058,7 @@
     </row>
     <row r="122" spans="66:71">
       <c r="BN122" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.5</v>
       </c>
       <c r="BO122" s="9" t="s">

</xml_diff>

<commit_message>
Revert "Added Sugar factory"
This reverts commit 036da8ab1cab1ca273227dc1a75a4cd3be3fbffb.
</commit_message>
<xml_diff>
--- a/Goods Production Calculator.xlsx
+++ b/Goods Production Calculator.xlsx
@@ -1,34 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78683BC6-204F-45EC-86CA-3DA9450FDDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Goods Price" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="146">
   <si>
     <t>small_arms</t>
   </si>
@@ -466,16 +454,13 @@
   </si>
   <si>
     <t>leather_fabric_factory</t>
-  </si>
-  <si>
-    <t>sugar_factory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,40 +616,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -706,7 +683,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,27 +715,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -790,24 +749,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -983,14 +924,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CG148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
-      <selection activeCell="BY65" sqref="BY65"/>
+    <sheetView tabSelected="1" topLeftCell="BI93" workbookViewId="0">
+      <selection activeCell="BQ108" sqref="BQ108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
@@ -1063,7 +1004,7 @@
     <col min="70" max="70" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="8.5703125" style="6" customWidth="1"/>
-    <col min="73" max="73" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="4" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -1078,7 +1019,7 @@
     <col min="85" max="85" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1046,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1135,7 +1076,7 @@
       <c r="M2" s="7"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1160,74 +1101,74 @@
         <v>0.3</v>
       </c>
       <c r="I3" s="6"/>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="R3" s="21" t="s">
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="R3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="Y3" s="21" t="s">
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="Y3" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AF3" s="21" t="s">
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AF3" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AM3" s="21" t="s">
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AM3" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="AN3" s="21"/>
-      <c r="AO3" s="21"/>
-      <c r="AP3" s="21"/>
-      <c r="AT3" s="21" t="s">
+      <c r="AN3" s="22"/>
+      <c r="AO3" s="22"/>
+      <c r="AP3" s="22"/>
+      <c r="AT3" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="AU3" s="21"/>
-      <c r="AV3" s="21"/>
-      <c r="AW3" s="21"/>
-      <c r="BA3" s="21" t="s">
+      <c r="AU3" s="22"/>
+      <c r="AV3" s="22"/>
+      <c r="AW3" s="22"/>
+      <c r="BA3" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="BB3" s="21"/>
-      <c r="BC3" s="21"/>
-      <c r="BD3" s="21"/>
-      <c r="BH3" s="21" t="s">
+      <c r="BB3" s="22"/>
+      <c r="BC3" s="22"/>
+      <c r="BD3" s="22"/>
+      <c r="BH3" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="BI3" s="21"/>
-      <c r="BJ3" s="21"/>
-      <c r="BK3" s="21"/>
-      <c r="BO3" s="21" t="s">
+      <c r="BI3" s="22"/>
+      <c r="BJ3" s="22"/>
+      <c r="BK3" s="22"/>
+      <c r="BO3" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="BP3" s="21"/>
-      <c r="BQ3" s="21"/>
-      <c r="BR3" s="21"/>
-      <c r="BV3" s="21" t="s">
+      <c r="BP3" s="22"/>
+      <c r="BQ3" s="22"/>
+      <c r="BR3" s="22"/>
+      <c r="BV3" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="BW3" s="21"/>
-      <c r="BX3" s="21"/>
-      <c r="BY3" s="21"/>
-      <c r="CC3" s="21" t="s">
+      <c r="BW3" s="22"/>
+      <c r="BX3" s="22"/>
+      <c r="BY3" s="22"/>
+      <c r="CC3" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="CD3" s="21"/>
-      <c r="CE3" s="21"/>
-      <c r="CF3" s="21"/>
-    </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="CD3" s="22"/>
+      <c r="CE3" s="22"/>
+      <c r="CF3" s="22"/>
+    </row>
+    <row r="4" spans="1:85">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1257,7 +1198,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1287,7 +1228,7 @@
       <c r="M5" s="7"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1317,7 +1258,7 @@
       <c r="M6" s="7"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1341,84 +1282,84 @@
       <c r="H7" s="3">
         <v>0</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="R7" s="20" t="s">
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="R7" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
       <c r="V7" s="5"/>
-      <c r="Y7" s="20" t="s">
+      <c r="Y7" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="20"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
       <c r="AC7" s="5"/>
-      <c r="AF7" s="20" t="s">
+      <c r="AF7" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="AG7" s="20"/>
-      <c r="AH7" s="20"/>
-      <c r="AI7" s="20"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="21"/>
+      <c r="AI7" s="21"/>
       <c r="AJ7" s="5"/>
-      <c r="AM7" s="20" t="s">
+      <c r="AM7" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="AN7" s="20"/>
-      <c r="AO7" s="20"/>
-      <c r="AP7" s="20"/>
+      <c r="AN7" s="21"/>
+      <c r="AO7" s="21"/>
+      <c r="AP7" s="21"/>
       <c r="AQ7" s="5"/>
-      <c r="AT7" s="20" t="s">
+      <c r="AT7" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="AU7" s="20"/>
-      <c r="AV7" s="20"/>
-      <c r="AW7" s="20"/>
+      <c r="AU7" s="21"/>
+      <c r="AV7" s="21"/>
+      <c r="AW7" s="21"/>
       <c r="AX7" s="5"/>
-      <c r="BA7" s="20" t="s">
+      <c r="BA7" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="BB7" s="20"/>
-      <c r="BC7" s="20"/>
-      <c r="BD7" s="20"/>
+      <c r="BB7" s="21"/>
+      <c r="BC7" s="21"/>
+      <c r="BD7" s="21"/>
       <c r="BE7" s="5"/>
-      <c r="BH7" s="20" t="s">
+      <c r="BH7" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="BI7" s="20"/>
-      <c r="BJ7" s="20"/>
-      <c r="BK7" s="20"/>
+      <c r="BI7" s="21"/>
+      <c r="BJ7" s="21"/>
+      <c r="BK7" s="21"/>
       <c r="BL7" s="5"/>
-      <c r="BO7" s="20" t="s">
+      <c r="BO7" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="BP7" s="20"/>
-      <c r="BQ7" s="20"/>
-      <c r="BR7" s="20"/>
+      <c r="BP7" s="21"/>
+      <c r="BQ7" s="21"/>
+      <c r="BR7" s="21"/>
       <c r="BS7" s="5"/>
-      <c r="BV7" s="20" t="s">
+      <c r="BV7" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="BW7" s="20"/>
-      <c r="BX7" s="20"/>
-      <c r="BY7" s="20"/>
+      <c r="BW7" s="21"/>
+      <c r="BX7" s="21"/>
+      <c r="BY7" s="21"/>
       <c r="BZ7" s="5"/>
-      <c r="CC7" s="20" t="s">
+      <c r="CC7" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="CD7" s="20"/>
-      <c r="CE7" s="20"/>
-      <c r="CF7" s="20"/>
+      <c r="CD7" s="21"/>
+      <c r="CE7" s="21"/>
+      <c r="CF7" s="21"/>
       <c r="CG7" s="5"/>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1593,7 +1534,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1823,7 +1764,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1926,7 +1867,7 @@
       <c r="CF10" s="10"/>
       <c r="CG10" s="5"/>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2030,7 +1971,7 @@
       <c r="CF11" s="10"/>
       <c r="CG11" s="5"/>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -2112,7 +2053,7 @@
       <c r="CF12" s="10"/>
       <c r="CG12" s="5"/>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2253,7 +2194,7 @@
       </c>
       <c r="CG13" s="5"/>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:85">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -2361,7 +2302,7 @@
       </c>
       <c r="CG14" s="5"/>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:85">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -2436,7 +2377,7 @@
       <c r="CD15" s="19"/>
       <c r="CG15" s="5"/>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -2511,7 +2452,7 @@
       </c>
       <c r="CG16" s="5"/>
     </row>
-    <row r="17" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:85">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -2521,7 +2462,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:85">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -2530,84 +2471,84 @@
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="R18" s="20" t="s">
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="R18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="S18" s="20"/>
-      <c r="T18" s="20"/>
-      <c r="U18" s="20"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
       <c r="V18" s="5"/>
-      <c r="Y18" s="20" t="s">
+      <c r="Y18" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="Z18" s="20"/>
-      <c r="AA18" s="20"/>
-      <c r="AB18" s="20"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+      <c r="AB18" s="21"/>
       <c r="AC18" s="5"/>
-      <c r="AF18" s="20" t="s">
+      <c r="AF18" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="AG18" s="20"/>
-      <c r="AH18" s="20"/>
-      <c r="AI18" s="20"/>
+      <c r="AG18" s="21"/>
+      <c r="AH18" s="21"/>
+      <c r="AI18" s="21"/>
       <c r="AJ18" s="5"/>
-      <c r="AM18" s="20" t="s">
+      <c r="AM18" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="AN18" s="20"/>
-      <c r="AO18" s="20"/>
-      <c r="AP18" s="20"/>
+      <c r="AN18" s="21"/>
+      <c r="AO18" s="21"/>
+      <c r="AP18" s="21"/>
       <c r="AQ18" s="5"/>
-      <c r="AT18" s="20" t="s">
+      <c r="AT18" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="AU18" s="20"/>
-      <c r="AV18" s="20"/>
-      <c r="AW18" s="20"/>
+      <c r="AU18" s="21"/>
+      <c r="AV18" s="21"/>
+      <c r="AW18" s="21"/>
       <c r="AX18" s="5"/>
-      <c r="BA18" s="20" t="s">
+      <c r="BA18" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="BB18" s="20"/>
-      <c r="BC18" s="20"/>
-      <c r="BD18" s="20"/>
+      <c r="BB18" s="21"/>
+      <c r="BC18" s="21"/>
+      <c r="BD18" s="21"/>
       <c r="BE18" s="5"/>
-      <c r="BH18" s="20" t="s">
+      <c r="BH18" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="BI18" s="20"/>
-      <c r="BJ18" s="20"/>
-      <c r="BK18" s="20"/>
+      <c r="BI18" s="21"/>
+      <c r="BJ18" s="21"/>
+      <c r="BK18" s="21"/>
       <c r="BL18" s="5"/>
-      <c r="BO18" s="20" t="s">
+      <c r="BO18" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="BP18" s="20"/>
-      <c r="BQ18" s="20"/>
-      <c r="BR18" s="20"/>
+      <c r="BP18" s="21"/>
+      <c r="BQ18" s="21"/>
+      <c r="BR18" s="21"/>
       <c r="BS18" s="5"/>
-      <c r="BV18" s="20" t="s">
+      <c r="BV18" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="BW18" s="20"/>
-      <c r="BX18" s="20"/>
-      <c r="BY18" s="20"/>
+      <c r="BW18" s="21"/>
+      <c r="BX18" s="21"/>
+      <c r="BY18" s="21"/>
       <c r="BZ18" s="5"/>
-      <c r="CC18" s="20" t="s">
+      <c r="CC18" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="CD18" s="20"/>
-      <c r="CE18" s="20"/>
-      <c r="CF18" s="20"/>
+      <c r="CD18" s="21"/>
+      <c r="CE18" s="21"/>
+      <c r="CF18" s="21"/>
       <c r="CG18" s="5"/>
     </row>
-    <row r="19" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:85">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -2782,7 +2723,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:85">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -3012,7 +2953,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:85">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -3136,7 +3077,7 @@
       <c r="CF21" s="10"/>
       <c r="CG21" s="5"/>
     </row>
-    <row r="22" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:85">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -3232,7 +3173,7 @@
       <c r="CF22" s="10"/>
       <c r="CG22" s="5"/>
     </row>
-    <row r="23" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:85">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -3321,7 +3262,7 @@
       <c r="CF23" s="10"/>
       <c r="CG23" s="5"/>
     </row>
-    <row r="24" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:85">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -3462,7 +3403,7 @@
       </c>
       <c r="CG24" s="5"/>
     </row>
-    <row r="25" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:85">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -3570,7 +3511,7 @@
       </c>
       <c r="CG25" s="5"/>
     </row>
-    <row r="26" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:85">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -3645,7 +3586,7 @@
       <c r="CD26" s="19"/>
       <c r="CG26" s="5"/>
     </row>
-    <row r="27" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:85">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -3720,7 +3661,7 @@
       </c>
       <c r="CG27" s="5"/>
     </row>
-    <row r="28" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:85">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -3730,7 +3671,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:85">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -3739,39 +3680,39 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="K29" s="20" t="s">
+      <c r="K29" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-      <c r="R29" s="20" t="s">
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="R29" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="S29" s="20"/>
-      <c r="T29" s="20"/>
-      <c r="U29" s="20"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
       <c r="V29" s="5"/>
-      <c r="Y29" s="20" t="s">
+      <c r="Y29" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="Z29" s="20"/>
-      <c r="AA29" s="20"/>
-      <c r="AB29" s="20"/>
+      <c r="Z29" s="21"/>
+      <c r="AA29" s="21"/>
+      <c r="AB29" s="21"/>
       <c r="AC29" s="5"/>
-      <c r="AF29" s="20" t="s">
+      <c r="AF29" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="AG29" s="20"/>
-      <c r="AH29" s="20"/>
-      <c r="AI29" s="20"/>
+      <c r="AG29" s="21"/>
+      <c r="AH29" s="21"/>
+      <c r="AI29" s="21"/>
       <c r="AJ29" s="5"/>
-      <c r="AM29" s="20" t="s">
+      <c r="AM29" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="AN29" s="20"/>
-      <c r="AO29" s="20"/>
-      <c r="AP29" s="20"/>
+      <c r="AN29" s="21"/>
+      <c r="AO29" s="21"/>
+      <c r="AP29" s="21"/>
       <c r="AQ29" s="5"/>
       <c r="AS29" s="7"/>
       <c r="AT29" s="23"/>
@@ -3779,12 +3720,12 @@
       <c r="AV29" s="23"/>
       <c r="AW29" s="23"/>
       <c r="AX29" s="7"/>
-      <c r="BA29" s="20" t="s">
+      <c r="BA29" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="BB29" s="20"/>
-      <c r="BC29" s="20"/>
-      <c r="BD29" s="20"/>
+      <c r="BB29" s="21"/>
+      <c r="BC29" s="21"/>
+      <c r="BD29" s="21"/>
       <c r="BE29" s="5"/>
       <c r="BG29" s="14"/>
       <c r="BH29" s="16"/>
@@ -3792,29 +3733,29 @@
       <c r="BJ29" s="16"/>
       <c r="BK29" s="16"/>
       <c r="BL29" s="14"/>
-      <c r="BO29" s="20" t="s">
+      <c r="BO29" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="BP29" s="20"/>
-      <c r="BQ29" s="20"/>
-      <c r="BR29" s="20"/>
+      <c r="BP29" s="21"/>
+      <c r="BQ29" s="21"/>
+      <c r="BR29" s="21"/>
       <c r="BS29" s="5"/>
-      <c r="BV29" s="20" t="s">
+      <c r="BV29" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="BW29" s="20"/>
-      <c r="BX29" s="20"/>
-      <c r="BY29" s="20"/>
+      <c r="BW29" s="21"/>
+      <c r="BX29" s="21"/>
+      <c r="BY29" s="21"/>
       <c r="BZ29" s="5"/>
-      <c r="CC29" s="20" t="s">
+      <c r="CC29" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="CD29" s="20"/>
-      <c r="CE29" s="20"/>
-      <c r="CF29" s="20"/>
+      <c r="CD29" s="21"/>
+      <c r="CE29" s="21"/>
+      <c r="CF29" s="21"/>
       <c r="CG29" s="5"/>
     </row>
-    <row r="30" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:85">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -3971,7 +3912,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:85">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -4173,7 +4114,7 @@
         <v>0.29793510324483785</v>
       </c>
     </row>
-    <row r="32" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:85">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -4283,7 +4224,7 @@
       <c r="CF32" s="10"/>
       <c r="CG32" s="5"/>
     </row>
-    <row r="33" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:85">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -4386,7 +4327,7 @@
       <c r="CF33" s="10"/>
       <c r="CG33" s="5"/>
     </row>
-    <row r="34" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:85">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -4468,7 +4409,7 @@
       <c r="CF34" s="10"/>
       <c r="CG34" s="5"/>
     </row>
-    <row r="35" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:85">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -4597,7 +4538,7 @@
       </c>
       <c r="CG35" s="5"/>
     </row>
-    <row r="36" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:85">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -4699,7 +4640,7 @@
       </c>
       <c r="CG36" s="5"/>
     </row>
-    <row r="37" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:85">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -4750,8 +4691,8 @@
       <c r="BB37" s="19"/>
       <c r="BE37" s="5"/>
       <c r="BG37" s="14"/>
-      <c r="BH37" s="22"/>
-      <c r="BI37" s="22"/>
+      <c r="BH37" s="24"/>
+      <c r="BI37" s="24"/>
       <c r="BJ37" s="14"/>
       <c r="BK37" s="14"/>
       <c r="BL37" s="14"/>
@@ -4774,7 +4715,7 @@
       <c r="CD37" s="19"/>
       <c r="CG37" s="5"/>
     </row>
-    <row r="38" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:85">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -4849,7 +4790,7 @@
       </c>
       <c r="CG38" s="5"/>
     </row>
-    <row r="39" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:85">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -4859,7 +4800,7 @@
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:85">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
@@ -4868,32 +4809,32 @@
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="K40" s="20" t="s">
+      <c r="K40" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="Y40" s="20" t="s">
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="Y40" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="Z40" s="20"/>
-      <c r="AA40" s="20"/>
-      <c r="AB40" s="20"/>
+      <c r="Z40" s="21"/>
+      <c r="AA40" s="21"/>
+      <c r="AB40" s="21"/>
       <c r="AC40" s="5"/>
-      <c r="AF40" s="20" t="s">
+      <c r="AF40" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="AG40" s="20"/>
-      <c r="AH40" s="20"/>
-      <c r="AI40" s="20"/>
+      <c r="AG40" s="21"/>
+      <c r="AH40" s="21"/>
+      <c r="AI40" s="21"/>
       <c r="AJ40" s="5"/>
-      <c r="AM40" s="20" t="s">
+      <c r="AM40" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="AN40" s="20"/>
-      <c r="AO40" s="20"/>
-      <c r="AP40" s="20"/>
+      <c r="AN40" s="21"/>
+      <c r="AO40" s="21"/>
+      <c r="AP40" s="21"/>
       <c r="AQ40" s="5"/>
       <c r="AS40" s="7"/>
       <c r="AT40" s="13"/>
@@ -4901,12 +4842,12 @@
       <c r="AV40" s="13"/>
       <c r="AW40" s="13"/>
       <c r="AX40" s="7"/>
-      <c r="BA40" s="20" t="s">
+      <c r="BA40" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="BB40" s="20"/>
-      <c r="BC40" s="20"/>
-      <c r="BD40" s="20"/>
+      <c r="BB40" s="21"/>
+      <c r="BC40" s="21"/>
+      <c r="BD40" s="21"/>
       <c r="BE40" s="5"/>
       <c r="BG40" s="7"/>
       <c r="BH40" s="13"/>
@@ -4914,29 +4855,29 @@
       <c r="BJ40" s="13"/>
       <c r="BK40" s="13"/>
       <c r="BL40" s="7"/>
-      <c r="BO40" s="20" t="s">
+      <c r="BO40" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="BP40" s="20"/>
-      <c r="BQ40" s="20"/>
-      <c r="BR40" s="20"/>
+      <c r="BP40" s="21"/>
+      <c r="BQ40" s="21"/>
+      <c r="BR40" s="21"/>
       <c r="BS40" s="5"/>
-      <c r="BV40" s="20" t="s">
+      <c r="BV40" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="BW40" s="20"/>
-      <c r="BX40" s="20"/>
-      <c r="BY40" s="20"/>
+      <c r="BW40" s="21"/>
+      <c r="BX40" s="21"/>
+      <c r="BY40" s="21"/>
       <c r="BZ40" s="5"/>
-      <c r="CC40" s="20" t="s">
+      <c r="CC40" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="CD40" s="20"/>
-      <c r="CE40" s="20"/>
-      <c r="CF40" s="20"/>
+      <c r="CD40" s="21"/>
+      <c r="CE40" s="21"/>
+      <c r="CF40" s="21"/>
       <c r="CG40" s="5"/>
     </row>
-    <row r="41" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:85">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
@@ -5078,7 +5019,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:85">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
@@ -5260,7 +5201,7 @@
         <v>0.26144455747711093</v>
       </c>
     </row>
-    <row r="43" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:85">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
@@ -5371,7 +5312,7 @@
       <c r="CF43" s="10"/>
       <c r="CG43" s="5"/>
     </row>
-    <row r="44" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:85">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
@@ -5468,7 +5409,7 @@
       <c r="CF44" s="10"/>
       <c r="CG44" s="5"/>
     </row>
-    <row r="45" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:85">
       <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
@@ -5544,7 +5485,7 @@
       <c r="CF45" s="10"/>
       <c r="CG45" s="5"/>
     </row>
-    <row r="46" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:85">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
@@ -5661,7 +5602,7 @@
       </c>
       <c r="CG46" s="5"/>
     </row>
-    <row r="47" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:85">
       <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
@@ -5754,7 +5695,7 @@
       </c>
       <c r="CG47" s="5"/>
     </row>
-    <row r="48" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:85">
       <c r="A48" s="3" t="s">
         <v>47</v>
       </c>
@@ -5823,7 +5764,7 @@
       <c r="CD48" s="19"/>
       <c r="CG48" s="5"/>
     </row>
-    <row r="49" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:85">
       <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
@@ -5892,7 +5833,7 @@
       </c>
       <c r="CG49" s="5"/>
     </row>
-    <row r="50" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:85">
       <c r="A50" s="3" t="s">
         <v>49</v>
       </c>
@@ -5902,7 +5843,7 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:85">
       <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
@@ -5911,49 +5852,49 @@
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="K51" s="20" t="s">
+      <c r="K51" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="Y51" s="20" t="s">
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="Y51" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="Z51" s="20"/>
-      <c r="AA51" s="20"/>
-      <c r="AB51" s="20"/>
+      <c r="Z51" s="21"/>
+      <c r="AA51" s="21"/>
+      <c r="AB51" s="21"/>
       <c r="AC51" s="5"/>
-      <c r="BA51" s="20" t="s">
+      <c r="BA51" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="BB51" s="20"/>
-      <c r="BC51" s="20"/>
-      <c r="BD51" s="20"/>
+      <c r="BB51" s="21"/>
+      <c r="BC51" s="21"/>
+      <c r="BD51" s="21"/>
       <c r="BE51" s="5"/>
-      <c r="BO51" s="20" t="s">
+      <c r="BO51" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="BP51" s="20"/>
-      <c r="BQ51" s="20"/>
-      <c r="BR51" s="20"/>
+      <c r="BP51" s="21"/>
+      <c r="BQ51" s="21"/>
+      <c r="BR51" s="21"/>
       <c r="BS51" s="5"/>
-      <c r="BV51" s="20" t="s">
+      <c r="BV51" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="BW51" s="20"/>
-      <c r="BX51" s="20"/>
-      <c r="BY51" s="20"/>
+      <c r="BW51" s="21"/>
+      <c r="BX51" s="21"/>
+      <c r="BY51" s="21"/>
       <c r="BZ51" s="5"/>
-      <c r="CC51" s="20" t="s">
+      <c r="CC51" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="CD51" s="20"/>
-      <c r="CE51" s="20"/>
-      <c r="CF51" s="20"/>
+      <c r="CD51" s="21"/>
+      <c r="CE51" s="21"/>
+      <c r="CF51" s="21"/>
       <c r="CG51" s="5"/>
     </row>
-    <row r="52" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:85">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
@@ -6053,7 +5994,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:85">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
@@ -6183,7 +6124,7 @@
         <v>0.27474267616785397</v>
       </c>
     </row>
-    <row r="54" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:85">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
@@ -6270,7 +6211,7 @@
       <c r="CF54" s="10"/>
       <c r="CG54" s="5"/>
     </row>
-    <row r="55" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:85">
       <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
@@ -6343,7 +6284,7 @@
       <c r="CF55" s="10"/>
       <c r="CG55" s="5"/>
     </row>
-    <row r="56" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:85">
       <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
@@ -6395,7 +6336,7 @@
       <c r="CF56" s="10"/>
       <c r="CG56" s="5"/>
     </row>
-    <row r="57" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:85">
       <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
@@ -6476,7 +6417,7 @@
       </c>
       <c r="CG57" s="5"/>
     </row>
-    <row r="58" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:85">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -6539,7 +6480,7 @@
       </c>
       <c r="CG58" s="5"/>
     </row>
-    <row r="59" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:85">
       <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
@@ -6584,7 +6525,7 @@
       <c r="CD59" s="19"/>
       <c r="CG59" s="5"/>
     </row>
-    <row r="60" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:85">
       <c r="A60" s="3" t="s">
         <v>59</v>
       </c>
@@ -6629,7 +6570,7 @@
       </c>
       <c r="CG60" s="5"/>
     </row>
-    <row r="61" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:85">
       <c r="A61" s="3" t="s">
         <v>60</v>
       </c>
@@ -6639,7 +6580,7 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:85">
       <c r="A62" s="3" t="s">
         <v>61</v>
       </c>
@@ -6648,42 +6589,35 @@
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
-      <c r="K62" s="20" t="s">
+      <c r="K62" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="L62" s="20"/>
-      <c r="M62" s="20"/>
-      <c r="N62" s="20"/>
-      <c r="Y62" s="20" t="s">
+      <c r="L62" s="21"/>
+      <c r="M62" s="21"/>
+      <c r="N62" s="21"/>
+      <c r="Y62" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="Z62" s="20"/>
-      <c r="AA62" s="20"/>
-      <c r="AB62" s="20"/>
+      <c r="Z62" s="21"/>
+      <c r="AA62" s="21"/>
+      <c r="AB62" s="21"/>
       <c r="AC62" s="5"/>
-      <c r="BO62" s="20" t="s">
+      <c r="BO62" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="BP62" s="20"/>
-      <c r="BQ62" s="20"/>
-      <c r="BR62" s="20"/>
+      <c r="BP62" s="21"/>
+      <c r="BQ62" s="21"/>
+      <c r="BR62" s="21"/>
       <c r="BS62" s="5"/>
-      <c r="BV62" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="BW62" s="20"/>
-      <c r="BX62" s="20"/>
-      <c r="BY62" s="20"/>
-      <c r="BZ62" s="5"/>
-      <c r="CC62" s="20" t="s">
+      <c r="CC62" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="CD62" s="20"/>
-      <c r="CE62" s="20"/>
-      <c r="CF62" s="20"/>
+      <c r="CD62" s="21"/>
+      <c r="CE62" s="21"/>
+      <c r="CF62" s="21"/>
       <c r="CG62" s="5"/>
     </row>
-    <row r="63" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:85">
       <c r="A63" s="3" t="s">
         <v>62</v>
       </c>
@@ -6737,21 +6671,6 @@
       <c r="BS63" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="BV63" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="BW63" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BX63" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="BY63" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="BZ63" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="CC63" s="9" t="s">
         <v>68</v>
       </c>
@@ -6768,7 +6687,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:85">
       <c r="J64" s="3">
         <f>VLOOKUP(K64,$A:$B,2,FALSE)</f>
         <v>1.4</v>
@@ -6829,26 +6748,6 @@
         <f>(BP68/BP69)-1</f>
         <v>0.25153374233128845</v>
       </c>
-      <c r="BU64" s="3">
-        <f>VLOOKUP(BV64,$A:$B,2,FALSE)</f>
-        <v>1.4</v>
-      </c>
-      <c r="BV64" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="BW64" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="BX64" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="BY64" s="10">
-        <v>2.6</v>
-      </c>
-      <c r="BZ64" s="11">
-        <f>(BW68/BW69)-1</f>
-        <v>0.25</v>
-      </c>
       <c r="CB64" s="3">
         <f>VLOOKUP(CC64,$A:$B,2,FALSE)</f>
         <v>3.5</v>
@@ -6870,7 +6769,7 @@
         <v>0.36425648021828105</v>
       </c>
     </row>
-    <row r="65" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="65" spans="10:85">
       <c r="J65" s="3">
         <f t="shared" ref="J65:J66" si="8">VLOOKUP(K65,$A:$B,2,FALSE)</f>
         <v>1.5</v>
@@ -6909,12 +6808,6 @@
       <c r="BQ65" s="10"/>
       <c r="BR65" s="10"/>
       <c r="BS65" s="5"/>
-      <c r="BU65" s="3"/>
-      <c r="BV65" s="9"/>
-      <c r="BW65" s="9"/>
-      <c r="BX65" s="10"/>
-      <c r="BY65" s="10"/>
-      <c r="BZ65" s="5"/>
       <c r="CB65" s="3">
         <f>VLOOKUP(CC65,$A:$B,2,FALSE)</f>
         <v>2.5</v>
@@ -6929,7 +6822,7 @@
       <c r="CF65" s="10"/>
       <c r="CG65" s="5"/>
     </row>
-    <row r="66" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="66" spans="10:85">
       <c r="J66" s="3">
         <f t="shared" si="8"/>
         <v>1.6</v>
@@ -6961,12 +6854,6 @@
       <c r="BQ66" s="10"/>
       <c r="BR66" s="10"/>
       <c r="BS66" s="5"/>
-      <c r="BU66" s="3"/>
-      <c r="BV66" s="9"/>
-      <c r="BW66" s="9"/>
-      <c r="BX66" s="10"/>
-      <c r="BY66" s="10"/>
-      <c r="BZ66" s="5"/>
       <c r="CB66" s="3">
         <f>VLOOKUP(CC66,$A:$B,2,FALSE)</f>
         <v>3</v>
@@ -6981,7 +6868,7 @@
       <c r="CF66" s="10"/>
       <c r="CG66" s="5"/>
     </row>
-    <row r="67" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="67" spans="10:85">
       <c r="J67" s="3"/>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
@@ -7006,12 +6893,6 @@
       <c r="BQ67" s="10"/>
       <c r="BR67" s="10"/>
       <c r="BS67" s="5"/>
-      <c r="BU67" s="3"/>
-      <c r="BV67" s="9"/>
-      <c r="BW67" s="9"/>
-      <c r="BX67" s="10"/>
-      <c r="BY67" s="10"/>
-      <c r="BZ67" s="5"/>
       <c r="CB67" s="3"/>
       <c r="CC67" s="9"/>
       <c r="CD67" s="9"/>
@@ -7019,7 +6900,7 @@
       <c r="CF67" s="10"/>
       <c r="CG67" s="5"/>
     </row>
-    <row r="68" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="68" spans="10:85">
       <c r="J68" s="3">
         <f>VLOOKUP(M64,$A:$B,2,FALSE)</f>
         <v>1.5</v>
@@ -7055,18 +6936,6 @@
         <v>44.88</v>
       </c>
       <c r="BS68" s="5"/>
-      <c r="BU68" s="3">
-        <f>VLOOKUP(BX64,$A:$B,2,FALSE)</f>
-        <v>2</v>
-      </c>
-      <c r="BV68" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BW68" s="3">
-        <f>SUM(BY64*BU68,BY65*BU69,BY66*BU70,BY67*BU71)</f>
-        <v>5.2</v>
-      </c>
-      <c r="BZ68" s="5"/>
       <c r="CB68" s="3">
         <f>VLOOKUP(CE64,$A:$B,2,FALSE)</f>
         <v>10</v>
@@ -7080,7 +6949,7 @@
       </c>
       <c r="CG68" s="5"/>
     </row>
-    <row r="69" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="69" spans="10:85">
       <c r="J69" s="3"/>
       <c r="K69" s="4" t="s">
         <v>73</v>
@@ -7107,15 +6976,6 @@
         <v>35.86</v>
       </c>
       <c r="BS69" s="5"/>
-      <c r="BU69" s="3"/>
-      <c r="BV69" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="BW69" s="3">
-        <f>SUM(BW64*BU64,BW65*BU65,BW66*BU66,BW67*BU67,BV71)</f>
-        <v>4.16</v>
-      </c>
-      <c r="BZ69" s="5"/>
       <c r="CB69" s="3"/>
       <c r="CC69" s="4" t="s">
         <v>73</v>
@@ -7126,7 +6986,7 @@
       </c>
       <c r="CG69" s="5"/>
     </row>
-    <row r="70" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="70" spans="10:85">
       <c r="J70" s="3"/>
       <c r="K70" s="18" t="s">
         <v>63</v>
@@ -7144,12 +7004,6 @@
       </c>
       <c r="BP70" s="19"/>
       <c r="BS70" s="5"/>
-      <c r="BU70" s="3"/>
-      <c r="BV70" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="BW70" s="19"/>
-      <c r="BZ70" s="5"/>
       <c r="CB70" s="3"/>
       <c r="CC70" s="18" t="s">
         <v>64</v>
@@ -7157,7 +7011,7 @@
       <c r="CD70" s="19"/>
       <c r="CG70" s="5"/>
     </row>
-    <row r="71" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="71" spans="10:85">
       <c r="J71" s="3"/>
       <c r="K71" s="3">
         <f>HLOOKUP(K70,$F$1:$H$6,6,FALSE)</f>
@@ -7175,12 +7029,6 @@
         <v>2.06</v>
       </c>
       <c r="BS71" s="5"/>
-      <c r="BU71" s="3"/>
-      <c r="BV71" s="3">
-        <f>HLOOKUP(BV70,$F$1:$H$6,6,FALSE)</f>
-        <v>2.06</v>
-      </c>
-      <c r="BZ71" s="5"/>
       <c r="CB71" s="3"/>
       <c r="CC71" s="3">
         <f>HLOOKUP(CC70,$F$1:$H$6,6,FALSE)</f>
@@ -7188,29 +7036,29 @@
       </c>
       <c r="CG71" s="5"/>
     </row>
-    <row r="73" spans="10:85" x14ac:dyDescent="0.25">
-      <c r="K73" s="20" t="s">
+    <row r="73" spans="10:85">
+      <c r="K73" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="L73" s="20"/>
-      <c r="M73" s="20"/>
-      <c r="N73" s="20"/>
-      <c r="Y73" s="20" t="s">
+      <c r="L73" s="21"/>
+      <c r="M73" s="21"/>
+      <c r="N73" s="21"/>
+      <c r="Y73" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="Z73" s="20"/>
-      <c r="AA73" s="20"/>
-      <c r="AB73" s="20"/>
+      <c r="Z73" s="21"/>
+      <c r="AA73" s="21"/>
+      <c r="AB73" s="21"/>
       <c r="AC73" s="5"/>
-      <c r="BO73" s="20" t="s">
+      <c r="BO73" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="BP73" s="20"/>
-      <c r="BQ73" s="20"/>
-      <c r="BR73" s="20"/>
+      <c r="BP73" s="21"/>
+      <c r="BQ73" s="21"/>
+      <c r="BR73" s="21"/>
       <c r="BS73" s="5"/>
     </row>
-    <row r="74" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="74" spans="10:85">
       <c r="K74" s="9" t="s">
         <v>68</v>
       </c>
@@ -7257,7 +7105,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="75" spans="10:85">
       <c r="J75" s="3">
         <f>VLOOKUP(K75,$A:$B,2,FALSE)</f>
         <v>1.4</v>
@@ -7319,7 +7167,7 @@
         <v>0.24641833810888247</v>
       </c>
     </row>
-    <row r="76" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="76" spans="10:85">
       <c r="J76" s="3">
         <f t="shared" ref="J76:J77" si="10">VLOOKUP(K76,$A:$B,2,FALSE)</f>
         <v>1.5</v>
@@ -7359,7 +7207,7 @@
       <c r="BR76" s="10"/>
       <c r="BS76" s="5"/>
     </row>
-    <row r="77" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="77" spans="10:85">
       <c r="J77" s="3">
         <f t="shared" si="10"/>
         <v>1.6</v>
@@ -7399,7 +7247,7 @@
       <c r="BR77" s="10"/>
       <c r="BS77" s="5"/>
     </row>
-    <row r="78" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="78" spans="10:85">
       <c r="J78" s="3"/>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
@@ -7425,7 +7273,7 @@
       <c r="BR78" s="10"/>
       <c r="BS78" s="5"/>
     </row>
-    <row r="79" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="79" spans="10:85">
       <c r="J79" s="3">
         <f>VLOOKUP(M75,$A:$B,2,FALSE)</f>
         <v>1.5</v>
@@ -7462,7 +7310,7 @@
       </c>
       <c r="BS79" s="5"/>
     </row>
-    <row r="80" spans="10:85" x14ac:dyDescent="0.25">
+    <row r="80" spans="10:85">
       <c r="J80" s="3"/>
       <c r="K80" s="4" t="s">
         <v>73</v>
@@ -7490,7 +7338,7 @@
       </c>
       <c r="BS80" s="5"/>
     </row>
-    <row r="81" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="81" spans="10:71">
       <c r="J81" s="3"/>
       <c r="K81" s="18" t="s">
         <v>63</v>
@@ -7509,7 +7357,7 @@
       <c r="BP81" s="19"/>
       <c r="BS81" s="5"/>
     </row>
-    <row r="82" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="82" spans="10:71">
       <c r="J82" s="3"/>
       <c r="K82" s="3">
         <f>HLOOKUP(K81,$F$1:$H$6,6,FALSE)</f>
@@ -7528,23 +7376,23 @@
       </c>
       <c r="BS82" s="5"/>
     </row>
-    <row r="84" spans="10:71" x14ac:dyDescent="0.25">
-      <c r="Y84" s="20" t="s">
+    <row r="84" spans="10:71">
+      <c r="Y84" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="Z84" s="20"/>
-      <c r="AA84" s="20"/>
-      <c r="AB84" s="20"/>
+      <c r="Z84" s="21"/>
+      <c r="AA84" s="21"/>
+      <c r="AB84" s="21"/>
       <c r="AC84" s="5"/>
-      <c r="BO84" s="20" t="s">
+      <c r="BO84" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="BP84" s="20"/>
-      <c r="BQ84" s="20"/>
-      <c r="BR84" s="20"/>
+      <c r="BP84" s="21"/>
+      <c r="BQ84" s="21"/>
+      <c r="BR84" s="21"/>
       <c r="BS84" s="5"/>
     </row>
-    <row r="85" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="85" spans="10:71">
       <c r="Y85" s="9" t="s">
         <v>68</v>
       </c>
@@ -7576,7 +7424,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="86" spans="10:71">
       <c r="X86" s="3">
         <f>VLOOKUP(Y86,$A:$B,2,FALSE)</f>
         <v>1.6</v>
@@ -7618,7 +7466,7 @@
         <v>0.24042879019908137</v>
       </c>
     </row>
-    <row r="87" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="87" spans="10:71">
       <c r="X87" s="3">
         <f>VLOOKUP(Y87,$A:$B,2,FALSE)</f>
         <v>1.8</v>
@@ -7646,7 +7494,7 @@
       <c r="BR87" s="10"/>
       <c r="BS87" s="5"/>
     </row>
-    <row r="88" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="88" spans="10:71">
       <c r="X88" s="3">
         <f>VLOOKUP(Y88,$A:$B,2,FALSE)</f>
         <v>5.2</v>
@@ -7674,7 +7522,7 @@
       <c r="BR88" s="10"/>
       <c r="BS88" s="5"/>
     </row>
-    <row r="89" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="89" spans="10:71">
       <c r="X89" s="3">
         <f>VLOOKUP(Y89,$A:$B,2,FALSE)</f>
         <v>2</v>
@@ -7695,7 +7543,7 @@
       <c r="BR89" s="10"/>
       <c r="BS89" s="5"/>
     </row>
-    <row r="90" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="90" spans="10:71">
       <c r="X90" s="3">
         <f>VLOOKUP(AA86,$A:$B,2,FALSE)</f>
         <v>4.3</v>
@@ -7721,7 +7569,7 @@
       </c>
       <c r="BS90" s="5"/>
     </row>
-    <row r="91" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="91" spans="10:71">
       <c r="X91" s="3"/>
       <c r="Y91" s="4" t="s">
         <v>73</v>
@@ -7741,7 +7589,7 @@
       </c>
       <c r="BS91" s="5"/>
     </row>
-    <row r="92" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="92" spans="10:71">
       <c r="X92" s="3"/>
       <c r="Y92" s="18" t="s">
         <v>63</v>
@@ -7755,7 +7603,7 @@
       <c r="BP92" s="19"/>
       <c r="BS92" s="5"/>
     </row>
-    <row r="93" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="93" spans="10:71">
       <c r="X93" s="3"/>
       <c r="Y93" s="3">
         <f>HLOOKUP(Y92,$F$1:$H$6,6,FALSE)</f>
@@ -7769,23 +7617,23 @@
       </c>
       <c r="BS93" s="5"/>
     </row>
-    <row r="95" spans="10:71" x14ac:dyDescent="0.25">
-      <c r="Y95" s="20" t="s">
+    <row r="95" spans="10:71">
+      <c r="Y95" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="Z95" s="20"/>
-      <c r="AA95" s="20"/>
-      <c r="AB95" s="20"/>
+      <c r="Z95" s="21"/>
+      <c r="AA95" s="21"/>
+      <c r="AB95" s="21"/>
       <c r="AC95" s="5"/>
-      <c r="BO95" s="20" t="s">
+      <c r="BO95" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="BP95" s="20"/>
-      <c r="BQ95" s="20"/>
-      <c r="BR95" s="20"/>
+      <c r="BP95" s="21"/>
+      <c r="BQ95" s="21"/>
+      <c r="BR95" s="21"/>
       <c r="BS95" s="5"/>
     </row>
-    <row r="96" spans="10:71" x14ac:dyDescent="0.25">
+    <row r="96" spans="10:71">
       <c r="Y96" s="9" t="s">
         <v>68</v>
       </c>
@@ -7817,7 +7665,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="97" spans="24:71">
       <c r="X97" s="3">
         <f>VLOOKUP(Y97,$A:$B,2,FALSE)</f>
         <v>3.3</v>
@@ -7859,7 +7707,7 @@
         <v>0.25547045951859948</v>
       </c>
     </row>
-    <row r="98" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="98" spans="24:71">
       <c r="X98" s="3">
         <f>VLOOKUP(Y98,$A:$B,2,FALSE)</f>
         <v>1.6</v>
@@ -7887,7 +7735,7 @@
       <c r="BR98" s="10"/>
       <c r="BS98" s="5"/>
     </row>
-    <row r="99" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="99" spans="24:71">
       <c r="X99" s="3">
         <f>VLOOKUP(Y99,$A:$B,2,FALSE)</f>
         <v>5.2</v>
@@ -7915,7 +7763,7 @@
       <c r="BR99" s="10"/>
       <c r="BS99" s="5"/>
     </row>
-    <row r="100" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="100" spans="24:71">
       <c r="X100" s="3"/>
       <c r="Y100" s="9"/>
       <c r="Z100" s="9"/>
@@ -7936,7 +7784,7 @@
       <c r="BR100" s="10"/>
       <c r="BS100" s="5"/>
     </row>
-    <row r="101" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="101" spans="24:71">
       <c r="X101" s="3">
         <f>VLOOKUP(AA97,$A:$B,2,FALSE)</f>
         <v>4.0999999999999996</v>
@@ -7962,7 +7810,7 @@
       </c>
       <c r="BS101" s="5"/>
     </row>
-    <row r="102" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="102" spans="24:71">
       <c r="X102" s="3"/>
       <c r="Y102" s="4" t="s">
         <v>73</v>
@@ -7982,7 +7830,7 @@
       </c>
       <c r="BS102" s="5"/>
     </row>
-    <row r="103" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="103" spans="24:71">
       <c r="X103" s="3"/>
       <c r="Y103" s="18" t="s">
         <v>63</v>
@@ -7996,7 +7844,7 @@
       <c r="BP103" s="19"/>
       <c r="BS103" s="5"/>
     </row>
-    <row r="104" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="104" spans="24:71">
       <c r="X104" s="3"/>
       <c r="Y104" s="3">
         <f>HLOOKUP(Y103,$F$1:$H$6,6,FALSE)</f>
@@ -8010,16 +7858,16 @@
       </c>
       <c r="BS104" s="5"/>
     </row>
-    <row r="106" spans="24:71" x14ac:dyDescent="0.25">
-      <c r="BO106" s="20" t="s">
+    <row r="106" spans="24:71">
+      <c r="BO106" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="BP106" s="20"/>
-      <c r="BQ106" s="20"/>
-      <c r="BR106" s="20"/>
+      <c r="BP106" s="21"/>
+      <c r="BQ106" s="21"/>
+      <c r="BR106" s="21"/>
       <c r="BS106" s="5"/>
     </row>
-    <row r="107" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="107" spans="24:71">
       <c r="BO107" s="9" t="s">
         <v>68</v>
       </c>
@@ -8036,7 +7884,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="108" spans="24:71">
       <c r="BN108" s="3">
         <f>VLOOKUP(BO108,$A:$B,2,FALSE)</f>
         <v>3.5</v>
@@ -8058,7 +7906,7 @@
         <v>0.22386537480877111</v>
       </c>
     </row>
-    <row r="109" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="109" spans="24:71">
       <c r="BN109" s="3">
         <f>VLOOKUP(BO109,$A:$B,2,FALSE)</f>
         <v>1.8</v>
@@ -8073,7 +7921,7 @@
       <c r="BR109" s="10"/>
       <c r="BS109" s="5"/>
     </row>
-    <row r="110" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="110" spans="24:71">
       <c r="BN110" s="3"/>
       <c r="BO110" s="9"/>
       <c r="BP110" s="9"/>
@@ -8081,7 +7929,7 @@
       <c r="BR110" s="10"/>
       <c r="BS110" s="5"/>
     </row>
-    <row r="111" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="111" spans="24:71">
       <c r="BN111" s="3"/>
       <c r="BO111" s="9"/>
       <c r="BP111" s="9"/>
@@ -8089,7 +7937,7 @@
       <c r="BR111" s="10"/>
       <c r="BS111" s="5"/>
     </row>
-    <row r="112" spans="24:71" x14ac:dyDescent="0.25">
+    <row r="112" spans="24:71">
       <c r="BN112" s="3">
         <f>VLOOKUP(BQ108,$A:$B,2,FALSE)</f>
         <v>4</v>
@@ -8103,7 +7951,7 @@
       </c>
       <c r="BS112" s="5"/>
     </row>
-    <row r="113" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="113" spans="66:71">
       <c r="BN113" s="3"/>
       <c r="BO113" s="4" t="s">
         <v>73</v>
@@ -8114,7 +7962,7 @@
       </c>
       <c r="BS113" s="5"/>
     </row>
-    <row r="114" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="114" spans="66:71">
       <c r="BN114" s="3"/>
       <c r="BO114" s="18" t="s">
         <v>63</v>
@@ -8122,7 +7970,7 @@
       <c r="BP114" s="19"/>
       <c r="BS114" s="5"/>
     </row>
-    <row r="115" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="115" spans="66:71">
       <c r="BN115" s="3"/>
       <c r="BO115" s="3">
         <f>HLOOKUP(BO114,$F$1:$H$6,6,FALSE)</f>
@@ -8130,16 +7978,16 @@
       </c>
       <c r="BS115" s="5"/>
     </row>
-    <row r="117" spans="66:71" x14ac:dyDescent="0.25">
-      <c r="BO117" s="20" t="s">
+    <row r="117" spans="66:71">
+      <c r="BO117" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="BP117" s="20"/>
-      <c r="BQ117" s="20"/>
-      <c r="BR117" s="20"/>
+      <c r="BP117" s="21"/>
+      <c r="BQ117" s="21"/>
+      <c r="BR117" s="21"/>
       <c r="BS117" s="5"/>
     </row>
-    <row r="118" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="118" spans="66:71">
       <c r="BO118" s="9" t="s">
         <v>68</v>
       </c>
@@ -8156,7 +8004,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="119" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="119" spans="66:71">
       <c r="BN119" s="3">
         <f>VLOOKUP(BO119,$A:$B,2,FALSE)</f>
         <v>3.2</v>
@@ -8178,7 +8026,7 @@
         <v>0.18955512572533828</v>
       </c>
     </row>
-    <row r="120" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="120" spans="66:71">
       <c r="BN120" s="3">
         <f t="shared" ref="BN120:BN122" si="12">VLOOKUP(BO120,$A:$B,2,FALSE)</f>
         <v>1.8</v>
@@ -8193,7 +8041,7 @@
       <c r="BR120" s="10"/>
       <c r="BS120" s="5"/>
     </row>
-    <row r="121" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="121" spans="66:71">
       <c r="BN121" s="3">
         <f t="shared" si="12"/>
         <v>5.2</v>
@@ -8208,7 +8056,7 @@
       <c r="BR121" s="10"/>
       <c r="BS121" s="5"/>
     </row>
-    <row r="122" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="122" spans="66:71">
       <c r="BN122" s="3">
         <f t="shared" si="12"/>
         <v>3.5</v>
@@ -8223,7 +8071,7 @@
       <c r="BR122" s="10"/>
       <c r="BS122" s="5"/>
     </row>
-    <row r="123" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="123" spans="66:71">
       <c r="BN123" s="3">
         <f>VLOOKUP(BQ119,$A:$B,2,FALSE)</f>
         <v>4.5</v>
@@ -8237,7 +8085,7 @@
       </c>
       <c r="BS123" s="5"/>
     </row>
-    <row r="124" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="124" spans="66:71">
       <c r="BN124" s="3"/>
       <c r="BO124" s="4" t="s">
         <v>73</v>
@@ -8248,7 +8096,7 @@
       </c>
       <c r="BS124" s="5"/>
     </row>
-    <row r="125" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="125" spans="66:71">
       <c r="BN125" s="3"/>
       <c r="BO125" s="18" t="s">
         <v>63</v>
@@ -8256,7 +8104,7 @@
       <c r="BP125" s="19"/>
       <c r="BS125" s="5"/>
     </row>
-    <row r="126" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="126" spans="66:71">
       <c r="BN126" s="3"/>
       <c r="BO126" s="3">
         <f>HLOOKUP(BO125,$F$1:$H$6,6,FALSE)</f>
@@ -8264,16 +8112,16 @@
       </c>
       <c r="BS126" s="5"/>
     </row>
-    <row r="128" spans="66:71" x14ac:dyDescent="0.25">
-      <c r="BO128" s="20" t="s">
+    <row r="128" spans="66:71">
+      <c r="BO128" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="BP128" s="20"/>
-      <c r="BQ128" s="20"/>
-      <c r="BR128" s="20"/>
+      <c r="BP128" s="21"/>
+      <c r="BQ128" s="21"/>
+      <c r="BR128" s="21"/>
       <c r="BS128" s="5"/>
     </row>
-    <row r="129" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="129" spans="66:71">
       <c r="BO129" s="9" t="s">
         <v>68</v>
       </c>
@@ -8290,7 +8138,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="130" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="130" spans="66:71">
       <c r="BN130" s="3">
         <f>VLOOKUP(BO130,$A:$B,2,FALSE)</f>
         <v>3.9</v>
@@ -8312,7 +8160,7 @@
         <v>0.22756640344580048</v>
       </c>
     </row>
-    <row r="131" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="131" spans="66:71">
       <c r="BN131" s="3">
         <f>VLOOKUP(BO131,$A:$B,2,FALSE)</f>
         <v>4.7</v>
@@ -8327,7 +8175,7 @@
       <c r="BR131" s="10"/>
       <c r="BS131" s="5"/>
     </row>
-    <row r="132" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="132" spans="66:71">
       <c r="BN132" s="3"/>
       <c r="BO132" s="9"/>
       <c r="BP132" s="9"/>
@@ -8335,7 +8183,7 @@
       <c r="BR132" s="10"/>
       <c r="BS132" s="5"/>
     </row>
-    <row r="133" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="133" spans="66:71">
       <c r="BN133" s="3"/>
       <c r="BO133" s="9"/>
       <c r="BP133" s="9"/>
@@ -8343,7 +8191,7 @@
       <c r="BR133" s="10"/>
       <c r="BS133" s="5"/>
     </row>
-    <row r="134" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="134" spans="66:71">
       <c r="BN134" s="3">
         <f>VLOOKUP(BQ130,$A:$B,2,FALSE)</f>
         <v>6</v>
@@ -8357,7 +8205,7 @@
       </c>
       <c r="BS134" s="5"/>
     </row>
-    <row r="135" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="135" spans="66:71">
       <c r="BN135" s="3"/>
       <c r="BO135" s="4" t="s">
         <v>73</v>
@@ -8368,7 +8216,7 @@
       </c>
       <c r="BS135" s="5"/>
     </row>
-    <row r="136" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="136" spans="66:71">
       <c r="BN136" s="3"/>
       <c r="BO136" s="18" t="s">
         <v>63</v>
@@ -8376,7 +8224,7 @@
       <c r="BP136" s="19"/>
       <c r="BS136" s="5"/>
     </row>
-    <row r="137" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="137" spans="66:71">
       <c r="BN137" s="3"/>
       <c r="BO137" s="3">
         <f>HLOOKUP(BO136,$F$1:$H$6,6,FALSE)</f>
@@ -8384,16 +8232,16 @@
       </c>
       <c r="BS137" s="5"/>
     </row>
-    <row r="139" spans="66:71" x14ac:dyDescent="0.25">
-      <c r="BO139" s="20" t="s">
+    <row r="139" spans="66:71">
+      <c r="BO139" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="BP139" s="20"/>
-      <c r="BQ139" s="20"/>
-      <c r="BR139" s="20"/>
+      <c r="BP139" s="21"/>
+      <c r="BQ139" s="21"/>
+      <c r="BR139" s="21"/>
       <c r="BS139" s="5"/>
     </row>
-    <row r="140" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="140" spans="66:71">
       <c r="BO140" s="9" t="s">
         <v>68</v>
       </c>
@@ -8410,7 +8258,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="141" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="141" spans="66:71">
       <c r="BN141" s="3">
         <f>VLOOKUP(BO141,$A:$B,2,FALSE)</f>
         <v>5.4</v>
@@ -8432,7 +8280,7 @@
         <v>0.26112759643916905</v>
       </c>
     </row>
-    <row r="142" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="142" spans="66:71">
       <c r="BN142" s="3">
         <f>VLOOKUP(BO142,$A:$B,2,FALSE)</f>
         <v>4.4000000000000004</v>
@@ -8447,7 +8295,7 @@
       <c r="BR142" s="10"/>
       <c r="BS142" s="5"/>
     </row>
-    <row r="143" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="143" spans="66:71">
       <c r="BN143" s="3">
         <f>VLOOKUP(BO143,$A:$B,2,FALSE)</f>
         <v>4.3</v>
@@ -8462,7 +8310,7 @@
       <c r="BR143" s="10"/>
       <c r="BS143" s="5"/>
     </row>
-    <row r="144" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="144" spans="66:71">
       <c r="BN144" s="3"/>
       <c r="BO144" s="9"/>
       <c r="BP144" s="9"/>
@@ -8470,7 +8318,7 @@
       <c r="BR144" s="10"/>
       <c r="BS144" s="5"/>
     </row>
-    <row r="145" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="145" spans="66:71">
       <c r="BN145" s="3">
         <f>VLOOKUP(BQ141,$A:$B,2,FALSE)</f>
         <v>4</v>
@@ -8484,7 +8332,7 @@
       </c>
       <c r="BS145" s="5"/>
     </row>
-    <row r="146" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="146" spans="66:71">
       <c r="BN146" s="3"/>
       <c r="BO146" s="4" t="s">
         <v>73</v>
@@ -8495,7 +8343,7 @@
       </c>
       <c r="BS146" s="5"/>
     </row>
-    <row r="147" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="147" spans="66:71">
       <c r="BN147" s="3"/>
       <c r="BO147" s="18" t="s">
         <v>63</v>
@@ -8503,7 +8351,7 @@
       <c r="BP147" s="19"/>
       <c r="BS147" s="5"/>
     </row>
-    <row r="148" spans="66:71" x14ac:dyDescent="0.25">
+    <row r="148" spans="66:71">
       <c r="BN148" s="3"/>
       <c r="BO148" s="3">
         <f>HLOOKUP(BO147,$F$1:$H$6,6,FALSE)</f>
@@ -8512,108 +8360,20 @@
       <c r="BS148" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="138">
-    <mergeCell ref="BV62:BY62"/>
-    <mergeCell ref="BV70:BW70"/>
-    <mergeCell ref="K81:L81"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="R29:U29"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="K62:N62"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="Y3:AB3"/>
-    <mergeCell ref="Y7:AB7"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y18:AB18"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y29:AB29"/>
-    <mergeCell ref="Y37:Z37"/>
-    <mergeCell ref="Y40:AB40"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="Y81:Z81"/>
-    <mergeCell ref="Y84:AB84"/>
-    <mergeCell ref="Y92:Z92"/>
-    <mergeCell ref="Y95:AB95"/>
-    <mergeCell ref="Y103:Z103"/>
-    <mergeCell ref="Y48:Z48"/>
-    <mergeCell ref="Y51:AB51"/>
-    <mergeCell ref="Y59:Z59"/>
-    <mergeCell ref="Y62:AB62"/>
-    <mergeCell ref="Y70:Z70"/>
-    <mergeCell ref="Y73:AB73"/>
-    <mergeCell ref="AF3:AI3"/>
-    <mergeCell ref="AF7:AI7"/>
-    <mergeCell ref="AF15:AG15"/>
-    <mergeCell ref="AF18:AI18"/>
-    <mergeCell ref="AF26:AG26"/>
-    <mergeCell ref="AF29:AI29"/>
-    <mergeCell ref="AF37:AG37"/>
-    <mergeCell ref="AF40:AI40"/>
-    <mergeCell ref="AF48:AG48"/>
-    <mergeCell ref="AM48:AN48"/>
-    <mergeCell ref="AT3:AW3"/>
-    <mergeCell ref="AT7:AW7"/>
-    <mergeCell ref="AT15:AU15"/>
-    <mergeCell ref="AT18:AW18"/>
-    <mergeCell ref="AT26:AU26"/>
-    <mergeCell ref="AT29:AW29"/>
-    <mergeCell ref="AT37:AU37"/>
-    <mergeCell ref="AT48:AU48"/>
-    <mergeCell ref="AM3:AP3"/>
-    <mergeCell ref="AM7:AP7"/>
-    <mergeCell ref="AM15:AN15"/>
-    <mergeCell ref="AM18:AP18"/>
-    <mergeCell ref="AM26:AN26"/>
-    <mergeCell ref="AM29:AP29"/>
-    <mergeCell ref="AM37:AN37"/>
-    <mergeCell ref="AM40:AP40"/>
-    <mergeCell ref="BA51:BD51"/>
-    <mergeCell ref="BA59:BB59"/>
-    <mergeCell ref="BH3:BK3"/>
-    <mergeCell ref="BH7:BK7"/>
-    <mergeCell ref="BH15:BI15"/>
-    <mergeCell ref="BH18:BK18"/>
-    <mergeCell ref="BH26:BI26"/>
-    <mergeCell ref="BA3:BD3"/>
-    <mergeCell ref="BA7:BD7"/>
-    <mergeCell ref="BA15:BB15"/>
-    <mergeCell ref="BA18:BD18"/>
-    <mergeCell ref="BA26:BB26"/>
-    <mergeCell ref="BA29:BD29"/>
-    <mergeCell ref="BO3:BR3"/>
-    <mergeCell ref="BO7:BR7"/>
-    <mergeCell ref="BO15:BP15"/>
-    <mergeCell ref="BO18:BR18"/>
-    <mergeCell ref="BO26:BP26"/>
-    <mergeCell ref="BO37:BP37"/>
-    <mergeCell ref="BO48:BP48"/>
-    <mergeCell ref="BA37:BB37"/>
-    <mergeCell ref="BA48:BB48"/>
-    <mergeCell ref="BA40:BD40"/>
-    <mergeCell ref="BO103:BP103"/>
-    <mergeCell ref="BO29:BR29"/>
-    <mergeCell ref="BO40:BR40"/>
-    <mergeCell ref="BO51:BR51"/>
-    <mergeCell ref="BO59:BP59"/>
-    <mergeCell ref="BO62:BR62"/>
-    <mergeCell ref="BO70:BP70"/>
-    <mergeCell ref="BH37:BI37"/>
-    <mergeCell ref="BH48:BI48"/>
+  <mergeCells count="136">
+    <mergeCell ref="CC70:CD70"/>
+    <mergeCell ref="CC48:CD48"/>
+    <mergeCell ref="CC29:CF29"/>
+    <mergeCell ref="CC40:CF40"/>
+    <mergeCell ref="CC51:CF51"/>
+    <mergeCell ref="CC59:CD59"/>
+    <mergeCell ref="CC62:CF62"/>
+    <mergeCell ref="CC3:CF3"/>
+    <mergeCell ref="CC7:CF7"/>
+    <mergeCell ref="CC15:CD15"/>
+    <mergeCell ref="CC18:CF18"/>
+    <mergeCell ref="CC26:CD26"/>
+    <mergeCell ref="CC37:CD37"/>
     <mergeCell ref="BV40:BY40"/>
     <mergeCell ref="BV51:BY51"/>
     <mergeCell ref="BV59:BW59"/>
@@ -8638,19 +8398,105 @@
     <mergeCell ref="BO84:BR84"/>
     <mergeCell ref="BO92:BP92"/>
     <mergeCell ref="BO95:BR95"/>
-    <mergeCell ref="CC70:CD70"/>
-    <mergeCell ref="CC48:CD48"/>
-    <mergeCell ref="CC29:CF29"/>
-    <mergeCell ref="CC40:CF40"/>
-    <mergeCell ref="CC51:CF51"/>
-    <mergeCell ref="CC59:CD59"/>
-    <mergeCell ref="CC62:CF62"/>
-    <mergeCell ref="CC3:CF3"/>
-    <mergeCell ref="CC7:CF7"/>
-    <mergeCell ref="CC15:CD15"/>
-    <mergeCell ref="CC18:CF18"/>
-    <mergeCell ref="CC26:CD26"/>
-    <mergeCell ref="CC37:CD37"/>
+    <mergeCell ref="BO103:BP103"/>
+    <mergeCell ref="BO29:BR29"/>
+    <mergeCell ref="BO40:BR40"/>
+    <mergeCell ref="BO51:BR51"/>
+    <mergeCell ref="BO59:BP59"/>
+    <mergeCell ref="BO62:BR62"/>
+    <mergeCell ref="BO70:BP70"/>
+    <mergeCell ref="BH37:BI37"/>
+    <mergeCell ref="BH48:BI48"/>
+    <mergeCell ref="BO3:BR3"/>
+    <mergeCell ref="BO7:BR7"/>
+    <mergeCell ref="BO15:BP15"/>
+    <mergeCell ref="BO18:BR18"/>
+    <mergeCell ref="BO26:BP26"/>
+    <mergeCell ref="BO37:BP37"/>
+    <mergeCell ref="BO48:BP48"/>
+    <mergeCell ref="BA37:BB37"/>
+    <mergeCell ref="BA48:BB48"/>
+    <mergeCell ref="BA40:BD40"/>
+    <mergeCell ref="BA51:BD51"/>
+    <mergeCell ref="BA59:BB59"/>
+    <mergeCell ref="BH3:BK3"/>
+    <mergeCell ref="BH7:BK7"/>
+    <mergeCell ref="BH15:BI15"/>
+    <mergeCell ref="BH18:BK18"/>
+    <mergeCell ref="BH26:BI26"/>
+    <mergeCell ref="BA3:BD3"/>
+    <mergeCell ref="BA7:BD7"/>
+    <mergeCell ref="BA15:BB15"/>
+    <mergeCell ref="BA18:BD18"/>
+    <mergeCell ref="BA26:BB26"/>
+    <mergeCell ref="BA29:BD29"/>
+    <mergeCell ref="AM48:AN48"/>
+    <mergeCell ref="AT3:AW3"/>
+    <mergeCell ref="AT7:AW7"/>
+    <mergeCell ref="AT15:AU15"/>
+    <mergeCell ref="AT18:AW18"/>
+    <mergeCell ref="AT26:AU26"/>
+    <mergeCell ref="AT29:AW29"/>
+    <mergeCell ref="AT37:AU37"/>
+    <mergeCell ref="AT48:AU48"/>
+    <mergeCell ref="AM3:AP3"/>
+    <mergeCell ref="AM7:AP7"/>
+    <mergeCell ref="AM15:AN15"/>
+    <mergeCell ref="AM18:AP18"/>
+    <mergeCell ref="AM26:AN26"/>
+    <mergeCell ref="AM29:AP29"/>
+    <mergeCell ref="AM37:AN37"/>
+    <mergeCell ref="AM40:AP40"/>
+    <mergeCell ref="AF3:AI3"/>
+    <mergeCell ref="AF7:AI7"/>
+    <mergeCell ref="AF15:AG15"/>
+    <mergeCell ref="AF18:AI18"/>
+    <mergeCell ref="AF26:AG26"/>
+    <mergeCell ref="AF29:AI29"/>
+    <mergeCell ref="AF37:AG37"/>
+    <mergeCell ref="AF40:AI40"/>
+    <mergeCell ref="AF48:AG48"/>
+    <mergeCell ref="Y81:Z81"/>
+    <mergeCell ref="Y84:AB84"/>
+    <mergeCell ref="Y92:Z92"/>
+    <mergeCell ref="Y95:AB95"/>
+    <mergeCell ref="Y103:Z103"/>
+    <mergeCell ref="Y48:Z48"/>
+    <mergeCell ref="Y51:AB51"/>
+    <mergeCell ref="Y59:Z59"/>
+    <mergeCell ref="Y62:AB62"/>
+    <mergeCell ref="Y70:Z70"/>
+    <mergeCell ref="Y73:AB73"/>
+    <mergeCell ref="Y3:AB3"/>
+    <mergeCell ref="Y7:AB7"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y18:AB18"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y29:AB29"/>
+    <mergeCell ref="Y37:Z37"/>
+    <mergeCell ref="Y40:AB40"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="R29:U29"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K37:L37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8658,19 +8504,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8678,7 +8524,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8686,7 +8532,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8694,7 +8540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -8702,7 +8548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -8710,7 +8556,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8718,7 +8564,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -8726,7 +8572,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -8734,7 +8580,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -8742,7 +8588,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -8750,7 +8596,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -8758,7 +8604,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -8766,7 +8612,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -8774,7 +8620,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -8782,7 +8628,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -8790,7 +8636,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -8798,7 +8644,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -8806,7 +8652,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -8814,7 +8660,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -8822,7 +8668,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -8830,7 +8676,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -8838,7 +8684,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -8846,7 +8692,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -8854,7 +8700,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -8862,7 +8708,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -8870,7 +8716,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -8878,7 +8724,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -8886,7 +8732,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -8894,7 +8740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -8902,7 +8748,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -8910,7 +8756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -8918,7 +8764,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -8926,7 +8772,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -8934,7 +8780,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -8942,7 +8788,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -8950,7 +8796,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -8958,7 +8804,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -8966,7 +8812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -8974,7 +8820,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -8982,7 +8828,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -8990,7 +8836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -8998,7 +8844,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -9006,7 +8852,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -9014,7 +8860,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -9022,7 +8868,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -9030,7 +8876,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -9038,7 +8884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -9046,7 +8892,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -9054,7 +8900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -9062,7 +8908,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -9070,7 +8916,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -9078,7 +8924,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -9086,7 +8932,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -9094,7 +8940,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -9102,7 +8948,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -9110,7 +8956,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -9118,7 +8964,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -9126,7 +8972,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -9134,7 +8980,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -9142,7 +8988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -9150,7 +8996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -9158,7 +9004,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -9166,7 +9012,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -9181,12 +9027,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Sugar factory - third try
</commit_message>
<xml_diff>
--- a/Goods Production Calculator.xlsx
+++ b/Goods Production Calculator.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A242AE-F6F4-42E4-92DA-C4BCFCAB5F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Goods Price" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="147">
   <si>
     <t>small_arms</t>
   </si>
@@ -454,13 +466,16 @@
   </si>
   <si>
     <t>leather_fabric_factory</t>
+  </si>
+  <si>
+    <t>sugar_factory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -616,32 +631,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -683,7 +706,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -715,9 +738,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -749,6 +790,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -924,14 +983,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI93" workbookViewId="0">
-      <selection activeCell="BQ108" sqref="BQ108"/>
+    <sheetView tabSelected="1" topLeftCell="BI45" workbookViewId="0">
+      <selection activeCell="BY65" sqref="BY65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
@@ -1019,7 +1078,7 @@
     <col min="85" max="85" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1105,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="5"/>
     </row>
-    <row r="2" spans="1:85">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1076,7 +1135,7 @@
       <c r="M2" s="7"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="1:85">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1101,74 +1160,74 @@
         <v>0.3</v>
       </c>
       <c r="I3" s="6"/>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="R3" s="22" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="R3" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="Y3" s="22" t="s">
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="Y3" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="Z3" s="22"/>
-      <c r="AA3" s="22"/>
-      <c r="AB3" s="22"/>
-      <c r="AF3" s="22" t="s">
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AF3" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="AG3" s="22"/>
-      <c r="AH3" s="22"/>
-      <c r="AI3" s="22"/>
-      <c r="AM3" s="22" t="s">
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AM3" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="AN3" s="22"/>
-      <c r="AO3" s="22"/>
-      <c r="AP3" s="22"/>
-      <c r="AT3" s="22" t="s">
+      <c r="AN3" s="21"/>
+      <c r="AO3" s="21"/>
+      <c r="AP3" s="21"/>
+      <c r="AT3" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="AU3" s="22"/>
-      <c r="AV3" s="22"/>
-      <c r="AW3" s="22"/>
-      <c r="BA3" s="22" t="s">
+      <c r="AU3" s="21"/>
+      <c r="AV3" s="21"/>
+      <c r="AW3" s="21"/>
+      <c r="BA3" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="BB3" s="22"/>
-      <c r="BC3" s="22"/>
-      <c r="BD3" s="22"/>
-      <c r="BH3" s="22" t="s">
+      <c r="BB3" s="21"/>
+      <c r="BC3" s="21"/>
+      <c r="BD3" s="21"/>
+      <c r="BH3" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="BI3" s="22"/>
-      <c r="BJ3" s="22"/>
-      <c r="BK3" s="22"/>
-      <c r="BO3" s="22" t="s">
+      <c r="BI3" s="21"/>
+      <c r="BJ3" s="21"/>
+      <c r="BK3" s="21"/>
+      <c r="BO3" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="BP3" s="22"/>
-      <c r="BQ3" s="22"/>
-      <c r="BR3" s="22"/>
-      <c r="BV3" s="22" t="s">
+      <c r="BP3" s="21"/>
+      <c r="BQ3" s="21"/>
+      <c r="BR3" s="21"/>
+      <c r="BV3" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="BW3" s="22"/>
-      <c r="BX3" s="22"/>
-      <c r="BY3" s="22"/>
-      <c r="CC3" s="22" t="s">
+      <c r="BW3" s="21"/>
+      <c r="BX3" s="21"/>
+      <c r="BY3" s="21"/>
+      <c r="CC3" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="CD3" s="22"/>
-      <c r="CE3" s="22"/>
-      <c r="CF3" s="22"/>
-    </row>
-    <row r="4" spans="1:85">
+      <c r="CD3" s="21"/>
+      <c r="CE3" s="21"/>
+      <c r="CF3" s="21"/>
+    </row>
+    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1198,7 +1257,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:85">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1228,7 +1287,7 @@
       <c r="M5" s="7"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:85">
+    <row r="6" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1258,7 +1317,7 @@
       <c r="M6" s="7"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:85">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1282,84 +1341,84 @@
       <c r="H7" s="3">
         <v>0</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="R7" s="21" t="s">
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="R7" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
       <c r="V7" s="5"/>
-      <c r="Y7" s="21" t="s">
+      <c r="Y7" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
       <c r="AC7" s="5"/>
-      <c r="AF7" s="21" t="s">
+      <c r="AF7" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="21"/>
-      <c r="AI7" s="21"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
       <c r="AJ7" s="5"/>
-      <c r="AM7" s="21" t="s">
+      <c r="AM7" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="AN7" s="21"/>
-      <c r="AO7" s="21"/>
-      <c r="AP7" s="21"/>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
       <c r="AQ7" s="5"/>
-      <c r="AT7" s="21" t="s">
+      <c r="AT7" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="AU7" s="21"/>
-      <c r="AV7" s="21"/>
-      <c r="AW7" s="21"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="20"/>
       <c r="AX7" s="5"/>
-      <c r="BA7" s="21" t="s">
+      <c r="BA7" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="BB7" s="21"/>
-      <c r="BC7" s="21"/>
-      <c r="BD7" s="21"/>
+      <c r="BB7" s="20"/>
+      <c r="BC7" s="20"/>
+      <c r="BD7" s="20"/>
       <c r="BE7" s="5"/>
-      <c r="BH7" s="21" t="s">
+      <c r="BH7" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="BI7" s="21"/>
-      <c r="BJ7" s="21"/>
-      <c r="BK7" s="21"/>
+      <c r="BI7" s="20"/>
+      <c r="BJ7" s="20"/>
+      <c r="BK7" s="20"/>
       <c r="BL7" s="5"/>
-      <c r="BO7" s="21" t="s">
+      <c r="BO7" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="BP7" s="21"/>
-      <c r="BQ7" s="21"/>
-      <c r="BR7" s="21"/>
+      <c r="BP7" s="20"/>
+      <c r="BQ7" s="20"/>
+      <c r="BR7" s="20"/>
       <c r="BS7" s="5"/>
-      <c r="BV7" s="21" t="s">
+      <c r="BV7" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="BW7" s="21"/>
-      <c r="BX7" s="21"/>
-      <c r="BY7" s="21"/>
+      <c r="BW7" s="20"/>
+      <c r="BX7" s="20"/>
+      <c r="BY7" s="20"/>
       <c r="BZ7" s="5"/>
-      <c r="CC7" s="21" t="s">
+      <c r="CC7" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="CD7" s="21"/>
-      <c r="CE7" s="21"/>
-      <c r="CF7" s="21"/>
+      <c r="CD7" s="20"/>
+      <c r="CE7" s="20"/>
+      <c r="CF7" s="20"/>
       <c r="CG7" s="5"/>
     </row>
-    <row r="8" spans="1:85">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1534,7 +1593,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:85">
+    <row r="9" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1764,7 +1823,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:85">
+    <row r="10" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1867,7 +1926,7 @@
       <c r="CF10" s="10"/>
       <c r="CG10" s="5"/>
     </row>
-    <row r="11" spans="1:85">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1971,7 +2030,7 @@
       <c r="CF11" s="10"/>
       <c r="CG11" s="5"/>
     </row>
-    <row r="12" spans="1:85">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -2053,7 +2112,7 @@
       <c r="CF12" s="10"/>
       <c r="CG12" s="5"/>
     </row>
-    <row r="13" spans="1:85">
+    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2194,7 +2253,7 @@
       </c>
       <c r="CG13" s="5"/>
     </row>
-    <row r="14" spans="1:85">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -2302,7 +2361,7 @@
       </c>
       <c r="CG14" s="5"/>
     </row>
-    <row r="15" spans="1:85">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -2377,7 +2436,7 @@
       <c r="CD15" s="19"/>
       <c r="CG15" s="5"/>
     </row>
-    <row r="16" spans="1:85">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -2452,7 +2511,7 @@
       </c>
       <c r="CG16" s="5"/>
     </row>
-    <row r="17" spans="1:85">
+    <row r="17" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -2462,7 +2521,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:85">
+    <row r="18" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -2471,84 +2530,84 @@
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="K18" s="21" t="s">
+      <c r="K18" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="R18" s="21" t="s">
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="R18" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
       <c r="V18" s="5"/>
-      <c r="Y18" s="21" t="s">
+      <c r="Y18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="21"/>
-      <c r="AB18" s="21"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
       <c r="AC18" s="5"/>
-      <c r="AF18" s="21" t="s">
+      <c r="AF18" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="AG18" s="21"/>
-      <c r="AH18" s="21"/>
-      <c r="AI18" s="21"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+      <c r="AI18" s="20"/>
       <c r="AJ18" s="5"/>
-      <c r="AM18" s="21" t="s">
+      <c r="AM18" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="AN18" s="21"/>
-      <c r="AO18" s="21"/>
-      <c r="AP18" s="21"/>
+      <c r="AN18" s="20"/>
+      <c r="AO18" s="20"/>
+      <c r="AP18" s="20"/>
       <c r="AQ18" s="5"/>
-      <c r="AT18" s="21" t="s">
+      <c r="AT18" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="AU18" s="21"/>
-      <c r="AV18" s="21"/>
-      <c r="AW18" s="21"/>
+      <c r="AU18" s="20"/>
+      <c r="AV18" s="20"/>
+      <c r="AW18" s="20"/>
       <c r="AX18" s="5"/>
-      <c r="BA18" s="21" t="s">
+      <c r="BA18" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="BB18" s="21"/>
-      <c r="BC18" s="21"/>
-      <c r="BD18" s="21"/>
+      <c r="BB18" s="20"/>
+      <c r="BC18" s="20"/>
+      <c r="BD18" s="20"/>
       <c r="BE18" s="5"/>
-      <c r="BH18" s="21" t="s">
+      <c r="BH18" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="BI18" s="21"/>
-      <c r="BJ18" s="21"/>
-      <c r="BK18" s="21"/>
+      <c r="BI18" s="20"/>
+      <c r="BJ18" s="20"/>
+      <c r="BK18" s="20"/>
       <c r="BL18" s="5"/>
-      <c r="BO18" s="21" t="s">
+      <c r="BO18" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="BP18" s="21"/>
-      <c r="BQ18" s="21"/>
-      <c r="BR18" s="21"/>
+      <c r="BP18" s="20"/>
+      <c r="BQ18" s="20"/>
+      <c r="BR18" s="20"/>
       <c r="BS18" s="5"/>
-      <c r="BV18" s="21" t="s">
+      <c r="BV18" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="BW18" s="21"/>
-      <c r="BX18" s="21"/>
-      <c r="BY18" s="21"/>
+      <c r="BW18" s="20"/>
+      <c r="BX18" s="20"/>
+      <c r="BY18" s="20"/>
       <c r="BZ18" s="5"/>
-      <c r="CC18" s="21" t="s">
+      <c r="CC18" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="CD18" s="21"/>
-      <c r="CE18" s="21"/>
-      <c r="CF18" s="21"/>
+      <c r="CD18" s="20"/>
+      <c r="CE18" s="20"/>
+      <c r="CF18" s="20"/>
       <c r="CG18" s="5"/>
     </row>
-    <row r="19" spans="1:85">
+    <row r="19" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -2723,7 +2782,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:85">
+    <row r="20" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -2953,7 +3012,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:85">
+    <row r="21" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -3077,7 +3136,7 @@
       <c r="CF21" s="10"/>
       <c r="CG21" s="5"/>
     </row>
-    <row r="22" spans="1:85">
+    <row r="22" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -3173,7 +3232,7 @@
       <c r="CF22" s="10"/>
       <c r="CG22" s="5"/>
     </row>
-    <row r="23" spans="1:85">
+    <row r="23" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -3262,7 +3321,7 @@
       <c r="CF23" s="10"/>
       <c r="CG23" s="5"/>
     </row>
-    <row r="24" spans="1:85">
+    <row r="24" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -3403,7 +3462,7 @@
       </c>
       <c r="CG24" s="5"/>
     </row>
-    <row r="25" spans="1:85">
+    <row r="25" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -3511,7 +3570,7 @@
       </c>
       <c r="CG25" s="5"/>
     </row>
-    <row r="26" spans="1:85">
+    <row r="26" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -3586,7 +3645,7 @@
       <c r="CD26" s="19"/>
       <c r="CG26" s="5"/>
     </row>
-    <row r="27" spans="1:85">
+    <row r="27" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -3661,7 +3720,7 @@
       </c>
       <c r="CG27" s="5"/>
     </row>
-    <row r="28" spans="1:85">
+    <row r="28" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -3671,7 +3730,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:85">
+    <row r="29" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -3680,39 +3739,39 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="K29" s="21" t="s">
+      <c r="K29" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="R29" s="21" t="s">
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="R29" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
-      <c r="U29" s="21"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="20"/>
       <c r="V29" s="5"/>
-      <c r="Y29" s="21" t="s">
+      <c r="Y29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="Z29" s="21"/>
-      <c r="AA29" s="21"/>
-      <c r="AB29" s="21"/>
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
       <c r="AC29" s="5"/>
-      <c r="AF29" s="21" t="s">
+      <c r="AF29" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="AG29" s="21"/>
-      <c r="AH29" s="21"/>
-      <c r="AI29" s="21"/>
+      <c r="AG29" s="20"/>
+      <c r="AH29" s="20"/>
+      <c r="AI29" s="20"/>
       <c r="AJ29" s="5"/>
-      <c r="AM29" s="21" t="s">
+      <c r="AM29" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="AN29" s="21"/>
-      <c r="AO29" s="21"/>
-      <c r="AP29" s="21"/>
+      <c r="AN29" s="20"/>
+      <c r="AO29" s="20"/>
+      <c r="AP29" s="20"/>
       <c r="AQ29" s="5"/>
       <c r="AS29" s="7"/>
       <c r="AT29" s="23"/>
@@ -3720,12 +3779,12 @@
       <c r="AV29" s="23"/>
       <c r="AW29" s="23"/>
       <c r="AX29" s="7"/>
-      <c r="BA29" s="21" t="s">
+      <c r="BA29" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="BB29" s="21"/>
-      <c r="BC29" s="21"/>
-      <c r="BD29" s="21"/>
+      <c r="BB29" s="20"/>
+      <c r="BC29" s="20"/>
+      <c r="BD29" s="20"/>
       <c r="BE29" s="5"/>
       <c r="BG29" s="14"/>
       <c r="BH29" s="16"/>
@@ -3733,29 +3792,29 @@
       <c r="BJ29" s="16"/>
       <c r="BK29" s="16"/>
       <c r="BL29" s="14"/>
-      <c r="BO29" s="21" t="s">
+      <c r="BO29" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="BP29" s="21"/>
-      <c r="BQ29" s="21"/>
-      <c r="BR29" s="21"/>
+      <c r="BP29" s="20"/>
+      <c r="BQ29" s="20"/>
+      <c r="BR29" s="20"/>
       <c r="BS29" s="5"/>
-      <c r="BV29" s="21" t="s">
+      <c r="BV29" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="BW29" s="21"/>
-      <c r="BX29" s="21"/>
-      <c r="BY29" s="21"/>
+      <c r="BW29" s="20"/>
+      <c r="BX29" s="20"/>
+      <c r="BY29" s="20"/>
       <c r="BZ29" s="5"/>
-      <c r="CC29" s="21" t="s">
+      <c r="CC29" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="CD29" s="21"/>
-      <c r="CE29" s="21"/>
-      <c r="CF29" s="21"/>
+      <c r="CD29" s="20"/>
+      <c r="CE29" s="20"/>
+      <c r="CF29" s="20"/>
       <c r="CG29" s="5"/>
     </row>
-    <row r="30" spans="1:85">
+    <row r="30" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -3912,7 +3971,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:85">
+    <row r="31" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -4114,7 +4173,7 @@
         <v>0.29793510324483785</v>
       </c>
     </row>
-    <row r="32" spans="1:85">
+    <row r="32" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -4224,7 +4283,7 @@
       <c r="CF32" s="10"/>
       <c r="CG32" s="5"/>
     </row>
-    <row r="33" spans="1:85">
+    <row r="33" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -4327,7 +4386,7 @@
       <c r="CF33" s="10"/>
       <c r="CG33" s="5"/>
     </row>
-    <row r="34" spans="1:85">
+    <row r="34" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -4409,7 +4468,7 @@
       <c r="CF34" s="10"/>
       <c r="CG34" s="5"/>
     </row>
-    <row r="35" spans="1:85">
+    <row r="35" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -4538,7 +4597,7 @@
       </c>
       <c r="CG35" s="5"/>
     </row>
-    <row r="36" spans="1:85">
+    <row r="36" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -4640,7 +4699,7 @@
       </c>
       <c r="CG36" s="5"/>
     </row>
-    <row r="37" spans="1:85">
+    <row r="37" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -4691,8 +4750,8 @@
       <c r="BB37" s="19"/>
       <c r="BE37" s="5"/>
       <c r="BG37" s="14"/>
-      <c r="BH37" s="24"/>
-      <c r="BI37" s="24"/>
+      <c r="BH37" s="22"/>
+      <c r="BI37" s="22"/>
       <c r="BJ37" s="14"/>
       <c r="BK37" s="14"/>
       <c r="BL37" s="14"/>
@@ -4715,7 +4774,7 @@
       <c r="CD37" s="19"/>
       <c r="CG37" s="5"/>
     </row>
-    <row r="38" spans="1:85">
+    <row r="38" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -4790,7 +4849,7 @@
       </c>
       <c r="CG38" s="5"/>
     </row>
-    <row r="39" spans="1:85">
+    <row r="39" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -4800,7 +4859,7 @@
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:85">
+    <row r="40" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
@@ -4809,32 +4868,32 @@
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
-      <c r="K40" s="21" t="s">
+      <c r="K40" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-      <c r="Y40" s="21" t="s">
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="Y40" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="Z40" s="21"/>
-      <c r="AA40" s="21"/>
-      <c r="AB40" s="21"/>
+      <c r="Z40" s="20"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="20"/>
       <c r="AC40" s="5"/>
-      <c r="AF40" s="21" t="s">
+      <c r="AF40" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="AG40" s="21"/>
-      <c r="AH40" s="21"/>
-      <c r="AI40" s="21"/>
+      <c r="AG40" s="20"/>
+      <c r="AH40" s="20"/>
+      <c r="AI40" s="20"/>
       <c r="AJ40" s="5"/>
-      <c r="AM40" s="21" t="s">
+      <c r="AM40" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="AN40" s="21"/>
-      <c r="AO40" s="21"/>
-      <c r="AP40" s="21"/>
+      <c r="AN40" s="20"/>
+      <c r="AO40" s="20"/>
+      <c r="AP40" s="20"/>
       <c r="AQ40" s="5"/>
       <c r="AS40" s="7"/>
       <c r="AT40" s="13"/>
@@ -4842,12 +4901,12 @@
       <c r="AV40" s="13"/>
       <c r="AW40" s="13"/>
       <c r="AX40" s="7"/>
-      <c r="BA40" s="21" t="s">
+      <c r="BA40" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="BB40" s="21"/>
-      <c r="BC40" s="21"/>
-      <c r="BD40" s="21"/>
+      <c r="BB40" s="20"/>
+      <c r="BC40" s="20"/>
+      <c r="BD40" s="20"/>
       <c r="BE40" s="5"/>
       <c r="BG40" s="7"/>
       <c r="BH40" s="13"/>
@@ -4855,29 +4914,29 @@
       <c r="BJ40" s="13"/>
       <c r="BK40" s="13"/>
       <c r="BL40" s="7"/>
-      <c r="BO40" s="21" t="s">
+      <c r="BO40" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="BP40" s="21"/>
-      <c r="BQ40" s="21"/>
-      <c r="BR40" s="21"/>
+      <c r="BP40" s="20"/>
+      <c r="BQ40" s="20"/>
+      <c r="BR40" s="20"/>
       <c r="BS40" s="5"/>
-      <c r="BV40" s="21" t="s">
+      <c r="BV40" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="BW40" s="21"/>
-      <c r="BX40" s="21"/>
-      <c r="BY40" s="21"/>
+      <c r="BW40" s="20"/>
+      <c r="BX40" s="20"/>
+      <c r="BY40" s="20"/>
       <c r="BZ40" s="5"/>
-      <c r="CC40" s="21" t="s">
+      <c r="CC40" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="CD40" s="21"/>
-      <c r="CE40" s="21"/>
-      <c r="CF40" s="21"/>
+      <c r="CD40" s="20"/>
+      <c r="CE40" s="20"/>
+      <c r="CF40" s="20"/>
       <c r="CG40" s="5"/>
     </row>
-    <row r="41" spans="1:85">
+    <row r="41" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
@@ -5019,7 +5078,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:85">
+    <row r="42" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
@@ -5201,7 +5260,7 @@
         <v>0.26144455747711093</v>
       </c>
     </row>
-    <row r="43" spans="1:85">
+    <row r="43" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
@@ -5312,7 +5371,7 @@
       <c r="CF43" s="10"/>
       <c r="CG43" s="5"/>
     </row>
-    <row r="44" spans="1:85">
+    <row r="44" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
@@ -5409,7 +5468,7 @@
       <c r="CF44" s="10"/>
       <c r="CG44" s="5"/>
     </row>
-    <row r="45" spans="1:85">
+    <row r="45" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
@@ -5485,7 +5544,7 @@
       <c r="CF45" s="10"/>
       <c r="CG45" s="5"/>
     </row>
-    <row r="46" spans="1:85">
+    <row r="46" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
@@ -5602,7 +5661,7 @@
       </c>
       <c r="CG46" s="5"/>
     </row>
-    <row r="47" spans="1:85">
+    <row r="47" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>46</v>
       </c>
@@ -5695,7 +5754,7 @@
       </c>
       <c r="CG47" s="5"/>
     </row>
-    <row r="48" spans="1:85">
+    <row r="48" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>47</v>
       </c>
@@ -5764,7 +5823,7 @@
       <c r="CD48" s="19"/>
       <c r="CG48" s="5"/>
     </row>
-    <row r="49" spans="1:85">
+    <row r="49" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
@@ -5833,7 +5892,7 @@
       </c>
       <c r="CG49" s="5"/>
     </row>
-    <row r="50" spans="1:85">
+    <row r="50" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>49</v>
       </c>
@@ -5843,7 +5902,7 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:85">
+    <row r="51" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
@@ -5852,49 +5911,49 @@
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="K51" s="21" t="s">
+      <c r="K51" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-      <c r="Y51" s="21" t="s">
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="Y51" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="Z51" s="21"/>
-      <c r="AA51" s="21"/>
-      <c r="AB51" s="21"/>
+      <c r="Z51" s="20"/>
+      <c r="AA51" s="20"/>
+      <c r="AB51" s="20"/>
       <c r="AC51" s="5"/>
-      <c r="BA51" s="21" t="s">
+      <c r="BA51" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="BB51" s="21"/>
-      <c r="BC51" s="21"/>
-      <c r="BD51" s="21"/>
+      <c r="BB51" s="20"/>
+      <c r="BC51" s="20"/>
+      <c r="BD51" s="20"/>
       <c r="BE51" s="5"/>
-      <c r="BO51" s="21" t="s">
+      <c r="BO51" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="BP51" s="21"/>
-      <c r="BQ51" s="21"/>
-      <c r="BR51" s="21"/>
+      <c r="BP51" s="20"/>
+      <c r="BQ51" s="20"/>
+      <c r="BR51" s="20"/>
       <c r="BS51" s="5"/>
-      <c r="BV51" s="21" t="s">
+      <c r="BV51" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="BW51" s="21"/>
-      <c r="BX51" s="21"/>
-      <c r="BY51" s="21"/>
+      <c r="BW51" s="20"/>
+      <c r="BX51" s="20"/>
+      <c r="BY51" s="20"/>
       <c r="BZ51" s="5"/>
-      <c r="CC51" s="21" t="s">
+      <c r="CC51" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="CD51" s="21"/>
-      <c r="CE51" s="21"/>
-      <c r="CF51" s="21"/>
+      <c r="CD51" s="20"/>
+      <c r="CE51" s="20"/>
+      <c r="CF51" s="20"/>
       <c r="CG51" s="5"/>
     </row>
-    <row r="52" spans="1:85">
+    <row r="52" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
@@ -5994,7 +6053,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:85">
+    <row r="53" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
@@ -6124,7 +6183,7 @@
         <v>0.27474267616785397</v>
       </c>
     </row>
-    <row r="54" spans="1:85">
+    <row r="54" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>53</v>
       </c>
@@ -6211,7 +6270,7 @@
       <c r="CF54" s="10"/>
       <c r="CG54" s="5"/>
     </row>
-    <row r="55" spans="1:85">
+    <row r="55" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>54</v>
       </c>
@@ -6284,7 +6343,7 @@
       <c r="CF55" s="10"/>
       <c r="CG55" s="5"/>
     </row>
-    <row r="56" spans="1:85">
+    <row r="56" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>55</v>
       </c>
@@ -6336,7 +6395,7 @@
       <c r="CF56" s="10"/>
       <c r="CG56" s="5"/>
     </row>
-    <row r="57" spans="1:85">
+    <row r="57" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
@@ -6417,7 +6476,7 @@
       </c>
       <c r="CG57" s="5"/>
     </row>
-    <row r="58" spans="1:85">
+    <row r="58" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>57</v>
       </c>
@@ -6480,7 +6539,7 @@
       </c>
       <c r="CG58" s="5"/>
     </row>
-    <row r="59" spans="1:85">
+    <row r="59" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
@@ -6525,7 +6584,7 @@
       <c r="CD59" s="19"/>
       <c r="CG59" s="5"/>
     </row>
-    <row r="60" spans="1:85">
+    <row r="60" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>59</v>
       </c>
@@ -6570,7 +6629,7 @@
       </c>
       <c r="CG60" s="5"/>
     </row>
-    <row r="61" spans="1:85">
+    <row r="61" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>60</v>
       </c>
@@ -6580,7 +6639,7 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:85">
+    <row r="62" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>61</v>
       </c>
@@ -6589,35 +6648,42 @@
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
-      <c r="K62" s="21" t="s">
+      <c r="K62" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="L62" s="21"/>
-      <c r="M62" s="21"/>
-      <c r="N62" s="21"/>
-      <c r="Y62" s="21" t="s">
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="Y62" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="Z62" s="21"/>
-      <c r="AA62" s="21"/>
-      <c r="AB62" s="21"/>
+      <c r="Z62" s="20"/>
+      <c r="AA62" s="20"/>
+      <c r="AB62" s="20"/>
       <c r="AC62" s="5"/>
-      <c r="BO62" s="21" t="s">
+      <c r="BO62" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="BP62" s="21"/>
-      <c r="BQ62" s="21"/>
-      <c r="BR62" s="21"/>
+      <c r="BP62" s="20"/>
+      <c r="BQ62" s="20"/>
+      <c r="BR62" s="20"/>
       <c r="BS62" s="5"/>
-      <c r="CC62" s="21" t="s">
+      <c r="BV62" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="BW62" s="20"/>
+      <c r="BX62" s="20"/>
+      <c r="BY62" s="20"/>
+      <c r="BZ62" s="5"/>
+      <c r="CC62" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="CD62" s="21"/>
-      <c r="CE62" s="21"/>
-      <c r="CF62" s="21"/>
+      <c r="CD62" s="20"/>
+      <c r="CE62" s="20"/>
+      <c r="CF62" s="20"/>
       <c r="CG62" s="5"/>
     </row>
-    <row r="63" spans="1:85">
+    <row r="63" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>62</v>
       </c>
@@ -6671,6 +6737,21 @@
       <c r="BS63" s="8" t="s">
         <v>70</v>
       </c>
+      <c r="BV63" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="BW63" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BX63" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="BY63" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="BZ63" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="CC63" s="9" t="s">
         <v>68</v>
       </c>
@@ -6687,7 +6768,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:85">
+    <row r="64" spans="1:85" x14ac:dyDescent="0.25">
       <c r="J64" s="3">
         <f>VLOOKUP(K64,$A:$B,2,FALSE)</f>
         <v>1.4</v>
@@ -6748,6 +6829,26 @@
         <f>(BP68/BP69)-1</f>
         <v>0.25153374233128845</v>
       </c>
+      <c r="BU64" s="3">
+        <f>VLOOKUP(BV64,$A:$B,2,FALSE)</f>
+        <v>1.4</v>
+      </c>
+      <c r="BV64" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW64" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="BX64" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="BY64" s="10">
+        <v>2.6</v>
+      </c>
+      <c r="BZ64" s="11">
+        <f>(BW68/BW69)-1</f>
+        <v>0.25</v>
+      </c>
       <c r="CB64" s="3">
         <f>VLOOKUP(CC64,$A:$B,2,FALSE)</f>
         <v>3.5</v>
@@ -6769,7 +6870,7 @@
         <v>0.36425648021828105</v>
       </c>
     </row>
-    <row r="65" spans="10:85">
+    <row r="65" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J65" s="3">
         <f t="shared" ref="J65:J66" si="8">VLOOKUP(K65,$A:$B,2,FALSE)</f>
         <v>1.5</v>
@@ -6808,6 +6909,12 @@
       <c r="BQ65" s="10"/>
       <c r="BR65" s="10"/>
       <c r="BS65" s="5"/>
+      <c r="BU65" s="3"/>
+      <c r="BV65" s="9"/>
+      <c r="BW65" s="9"/>
+      <c r="BX65" s="10"/>
+      <c r="BY65" s="10"/>
+      <c r="BZ65" s="5"/>
       <c r="CB65" s="3">
         <f>VLOOKUP(CC65,$A:$B,2,FALSE)</f>
         <v>2.5</v>
@@ -6822,7 +6929,7 @@
       <c r="CF65" s="10"/>
       <c r="CG65" s="5"/>
     </row>
-    <row r="66" spans="10:85">
+    <row r="66" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J66" s="3">
         <f t="shared" si="8"/>
         <v>1.6</v>
@@ -6854,6 +6961,12 @@
       <c r="BQ66" s="10"/>
       <c r="BR66" s="10"/>
       <c r="BS66" s="5"/>
+      <c r="BU66" s="3"/>
+      <c r="BV66" s="9"/>
+      <c r="BW66" s="9"/>
+      <c r="BX66" s="10"/>
+      <c r="BY66" s="10"/>
+      <c r="BZ66" s="5"/>
       <c r="CB66" s="3">
         <f>VLOOKUP(CC66,$A:$B,2,FALSE)</f>
         <v>3</v>
@@ -6868,7 +6981,7 @@
       <c r="CF66" s="10"/>
       <c r="CG66" s="5"/>
     </row>
-    <row r="67" spans="10:85">
+    <row r="67" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J67" s="3"/>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
@@ -6893,6 +7006,12 @@
       <c r="BQ67" s="10"/>
       <c r="BR67" s="10"/>
       <c r="BS67" s="5"/>
+      <c r="BU67" s="3"/>
+      <c r="BV67" s="9"/>
+      <c r="BW67" s="9"/>
+      <c r="BX67" s="10"/>
+      <c r="BY67" s="10"/>
+      <c r="BZ67" s="5"/>
       <c r="CB67" s="3"/>
       <c r="CC67" s="9"/>
       <c r="CD67" s="9"/>
@@ -6900,7 +7019,7 @@
       <c r="CF67" s="10"/>
       <c r="CG67" s="5"/>
     </row>
-    <row r="68" spans="10:85">
+    <row r="68" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J68" s="3">
         <f>VLOOKUP(M64,$A:$B,2,FALSE)</f>
         <v>1.5</v>
@@ -6936,6 +7055,18 @@
         <v>44.88</v>
       </c>
       <c r="BS68" s="5"/>
+      <c r="BU68" s="3">
+        <f>VLOOKUP(BX64,$A:$B,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="BV68" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="BW68" s="3">
+        <f>SUM(BY64*BU68,BY65*BU69,BY66*BU70,BY67*BU71)</f>
+        <v>5.2</v>
+      </c>
+      <c r="BZ68" s="5"/>
       <c r="CB68" s="3">
         <f>VLOOKUP(CE64,$A:$B,2,FALSE)</f>
         <v>10</v>
@@ -6949,7 +7080,7 @@
       </c>
       <c r="CG68" s="5"/>
     </row>
-    <row r="69" spans="10:85">
+    <row r="69" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J69" s="3"/>
       <c r="K69" s="4" t="s">
         <v>73</v>
@@ -6976,6 +7107,15 @@
         <v>35.86</v>
       </c>
       <c r="BS69" s="5"/>
+      <c r="BU69" s="3"/>
+      <c r="BV69" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW69" s="3">
+        <f>SUM(BW64*BU64,BW65*BU65,BW66*BU66,BW67*BU67,BV71)</f>
+        <v>4.16</v>
+      </c>
+      <c r="BZ69" s="5"/>
       <c r="CB69" s="3"/>
       <c r="CC69" s="4" t="s">
         <v>73</v>
@@ -6986,7 +7126,7 @@
       </c>
       <c r="CG69" s="5"/>
     </row>
-    <row r="70" spans="10:85">
+    <row r="70" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J70" s="3"/>
       <c r="K70" s="18" t="s">
         <v>63</v>
@@ -7004,6 +7144,12 @@
       </c>
       <c r="BP70" s="19"/>
       <c r="BS70" s="5"/>
+      <c r="BU70" s="3"/>
+      <c r="BV70" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BW70" s="19"/>
+      <c r="BZ70" s="5"/>
       <c r="CB70" s="3"/>
       <c r="CC70" s="18" t="s">
         <v>64</v>
@@ -7011,7 +7157,7 @@
       <c r="CD70" s="19"/>
       <c r="CG70" s="5"/>
     </row>
-    <row r="71" spans="10:85">
+    <row r="71" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J71" s="3"/>
       <c r="K71" s="3">
         <f>HLOOKUP(K70,$F$1:$H$6,6,FALSE)</f>
@@ -7029,6 +7175,12 @@
         <v>2.06</v>
       </c>
       <c r="BS71" s="5"/>
+      <c r="BU71" s="3"/>
+      <c r="BV71" s="3">
+        <f>HLOOKUP(BV70,$F$1:$H$6,6,FALSE)</f>
+        <v>2.06</v>
+      </c>
+      <c r="BZ71" s="5"/>
       <c r="CB71" s="3"/>
       <c r="CC71" s="3">
         <f>HLOOKUP(CC70,$F$1:$H$6,6,FALSE)</f>
@@ -7036,29 +7188,29 @@
       </c>
       <c r="CG71" s="5"/>
     </row>
-    <row r="73" spans="10:85">
-      <c r="K73" s="21" t="s">
+    <row r="73" spans="10:85" x14ac:dyDescent="0.25">
+      <c r="K73" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="L73" s="21"/>
-      <c r="M73" s="21"/>
-      <c r="N73" s="21"/>
-      <c r="Y73" s="21" t="s">
+      <c r="L73" s="20"/>
+      <c r="M73" s="20"/>
+      <c r="N73" s="20"/>
+      <c r="Y73" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="Z73" s="21"/>
-      <c r="AA73" s="21"/>
-      <c r="AB73" s="21"/>
+      <c r="Z73" s="20"/>
+      <c r="AA73" s="20"/>
+      <c r="AB73" s="20"/>
       <c r="AC73" s="5"/>
-      <c r="BO73" s="21" t="s">
+      <c r="BO73" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="BP73" s="21"/>
-      <c r="BQ73" s="21"/>
-      <c r="BR73" s="21"/>
+      <c r="BP73" s="20"/>
+      <c r="BQ73" s="20"/>
+      <c r="BR73" s="20"/>
       <c r="BS73" s="5"/>
     </row>
-    <row r="74" spans="10:85">
+    <row r="74" spans="10:85" x14ac:dyDescent="0.25">
       <c r="K74" s="9" t="s">
         <v>68</v>
       </c>
@@ -7105,7 +7257,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="10:85">
+    <row r="75" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J75" s="3">
         <f>VLOOKUP(K75,$A:$B,2,FALSE)</f>
         <v>1.4</v>
@@ -7167,7 +7319,7 @@
         <v>0.24641833810888247</v>
       </c>
     </row>
-    <row r="76" spans="10:85">
+    <row r="76" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J76" s="3">
         <f t="shared" ref="J76:J77" si="10">VLOOKUP(K76,$A:$B,2,FALSE)</f>
         <v>1.5</v>
@@ -7207,7 +7359,7 @@
       <c r="BR76" s="10"/>
       <c r="BS76" s="5"/>
     </row>
-    <row r="77" spans="10:85">
+    <row r="77" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J77" s="3">
         <f t="shared" si="10"/>
         <v>1.6</v>
@@ -7247,7 +7399,7 @@
       <c r="BR77" s="10"/>
       <c r="BS77" s="5"/>
     </row>
-    <row r="78" spans="10:85">
+    <row r="78" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J78" s="3"/>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
@@ -7273,7 +7425,7 @@
       <c r="BR78" s="10"/>
       <c r="BS78" s="5"/>
     </row>
-    <row r="79" spans="10:85">
+    <row r="79" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J79" s="3">
         <f>VLOOKUP(M75,$A:$B,2,FALSE)</f>
         <v>1.5</v>
@@ -7310,7 +7462,7 @@
       </c>
       <c r="BS79" s="5"/>
     </row>
-    <row r="80" spans="10:85">
+    <row r="80" spans="10:85" x14ac:dyDescent="0.25">
       <c r="J80" s="3"/>
       <c r="K80" s="4" t="s">
         <v>73</v>
@@ -7338,7 +7490,7 @@
       </c>
       <c r="BS80" s="5"/>
     </row>
-    <row r="81" spans="10:71">
+    <row r="81" spans="10:71" x14ac:dyDescent="0.25">
       <c r="J81" s="3"/>
       <c r="K81" s="18" t="s">
         <v>63</v>
@@ -7357,7 +7509,7 @@
       <c r="BP81" s="19"/>
       <c r="BS81" s="5"/>
     </row>
-    <row r="82" spans="10:71">
+    <row r="82" spans="10:71" x14ac:dyDescent="0.25">
       <c r="J82" s="3"/>
       <c r="K82" s="3">
         <f>HLOOKUP(K81,$F$1:$H$6,6,FALSE)</f>
@@ -7376,23 +7528,23 @@
       </c>
       <c r="BS82" s="5"/>
     </row>
-    <row r="84" spans="10:71">
-      <c r="Y84" s="21" t="s">
+    <row r="84" spans="10:71" x14ac:dyDescent="0.25">
+      <c r="Y84" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="Z84" s="21"/>
-      <c r="AA84" s="21"/>
-      <c r="AB84" s="21"/>
+      <c r="Z84" s="20"/>
+      <c r="AA84" s="20"/>
+      <c r="AB84" s="20"/>
       <c r="AC84" s="5"/>
-      <c r="BO84" s="21" t="s">
+      <c r="BO84" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="BP84" s="21"/>
-      <c r="BQ84" s="21"/>
-      <c r="BR84" s="21"/>
+      <c r="BP84" s="20"/>
+      <c r="BQ84" s="20"/>
+      <c r="BR84" s="20"/>
       <c r="BS84" s="5"/>
     </row>
-    <row r="85" spans="10:71">
+    <row r="85" spans="10:71" x14ac:dyDescent="0.25">
       <c r="Y85" s="9" t="s">
         <v>68</v>
       </c>
@@ -7424,7 +7576,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="10:71">
+    <row r="86" spans="10:71" x14ac:dyDescent="0.25">
       <c r="X86" s="3">
         <f>VLOOKUP(Y86,$A:$B,2,FALSE)</f>
         <v>1.6</v>
@@ -7466,7 +7618,7 @@
         <v>0.24042879019908137</v>
       </c>
     </row>
-    <row r="87" spans="10:71">
+    <row r="87" spans="10:71" x14ac:dyDescent="0.25">
       <c r="X87" s="3">
         <f>VLOOKUP(Y87,$A:$B,2,FALSE)</f>
         <v>1.8</v>
@@ -7494,7 +7646,7 @@
       <c r="BR87" s="10"/>
       <c r="BS87" s="5"/>
     </row>
-    <row r="88" spans="10:71">
+    <row r="88" spans="10:71" x14ac:dyDescent="0.25">
       <c r="X88" s="3">
         <f>VLOOKUP(Y88,$A:$B,2,FALSE)</f>
         <v>5.2</v>
@@ -7522,7 +7674,7 @@
       <c r="BR88" s="10"/>
       <c r="BS88" s="5"/>
     </row>
-    <row r="89" spans="10:71">
+    <row r="89" spans="10:71" x14ac:dyDescent="0.25">
       <c r="X89" s="3">
         <f>VLOOKUP(Y89,$A:$B,2,FALSE)</f>
         <v>2</v>
@@ -7543,7 +7695,7 @@
       <c r="BR89" s="10"/>
       <c r="BS89" s="5"/>
     </row>
-    <row r="90" spans="10:71">
+    <row r="90" spans="10:71" x14ac:dyDescent="0.25">
       <c r="X90" s="3">
         <f>VLOOKUP(AA86,$A:$B,2,FALSE)</f>
         <v>4.3</v>
@@ -7569,7 +7721,7 @@
       </c>
       <c r="BS90" s="5"/>
     </row>
-    <row r="91" spans="10:71">
+    <row r="91" spans="10:71" x14ac:dyDescent="0.25">
       <c r="X91" s="3"/>
       <c r="Y91" s="4" t="s">
         <v>73</v>
@@ -7589,7 +7741,7 @@
       </c>
       <c r="BS91" s="5"/>
     </row>
-    <row r="92" spans="10:71">
+    <row r="92" spans="10:71" x14ac:dyDescent="0.25">
       <c r="X92" s="3"/>
       <c r="Y92" s="18" t="s">
         <v>63</v>
@@ -7603,7 +7755,7 @@
       <c r="BP92" s="19"/>
       <c r="BS92" s="5"/>
     </row>
-    <row r="93" spans="10:71">
+    <row r="93" spans="10:71" x14ac:dyDescent="0.25">
       <c r="X93" s="3"/>
       <c r="Y93" s="3">
         <f>HLOOKUP(Y92,$F$1:$H$6,6,FALSE)</f>
@@ -7617,23 +7769,23 @@
       </c>
       <c r="BS93" s="5"/>
     </row>
-    <row r="95" spans="10:71">
-      <c r="Y95" s="21" t="s">
+    <row r="95" spans="10:71" x14ac:dyDescent="0.25">
+      <c r="Y95" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="Z95" s="21"/>
-      <c r="AA95" s="21"/>
-      <c r="AB95" s="21"/>
+      <c r="Z95" s="20"/>
+      <c r="AA95" s="20"/>
+      <c r="AB95" s="20"/>
       <c r="AC95" s="5"/>
-      <c r="BO95" s="21" t="s">
+      <c r="BO95" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="BP95" s="21"/>
-      <c r="BQ95" s="21"/>
-      <c r="BR95" s="21"/>
+      <c r="BP95" s="20"/>
+      <c r="BQ95" s="20"/>
+      <c r="BR95" s="20"/>
       <c r="BS95" s="5"/>
     </row>
-    <row r="96" spans="10:71">
+    <row r="96" spans="10:71" x14ac:dyDescent="0.25">
       <c r="Y96" s="9" t="s">
         <v>68</v>
       </c>
@@ -7665,7 +7817,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="24:71">
+    <row r="97" spans="24:71" x14ac:dyDescent="0.25">
       <c r="X97" s="3">
         <f>VLOOKUP(Y97,$A:$B,2,FALSE)</f>
         <v>3.3</v>
@@ -7707,7 +7859,7 @@
         <v>0.25547045951859948</v>
       </c>
     </row>
-    <row r="98" spans="24:71">
+    <row r="98" spans="24:71" x14ac:dyDescent="0.25">
       <c r="X98" s="3">
         <f>VLOOKUP(Y98,$A:$B,2,FALSE)</f>
         <v>1.6</v>
@@ -7735,7 +7887,7 @@
       <c r="BR98" s="10"/>
       <c r="BS98" s="5"/>
     </row>
-    <row r="99" spans="24:71">
+    <row r="99" spans="24:71" x14ac:dyDescent="0.25">
       <c r="X99" s="3">
         <f>VLOOKUP(Y99,$A:$B,2,FALSE)</f>
         <v>5.2</v>
@@ -7763,7 +7915,7 @@
       <c r="BR99" s="10"/>
       <c r="BS99" s="5"/>
     </row>
-    <row r="100" spans="24:71">
+    <row r="100" spans="24:71" x14ac:dyDescent="0.25">
       <c r="X100" s="3"/>
       <c r="Y100" s="9"/>
       <c r="Z100" s="9"/>
@@ -7784,7 +7936,7 @@
       <c r="BR100" s="10"/>
       <c r="BS100" s="5"/>
     </row>
-    <row r="101" spans="24:71">
+    <row r="101" spans="24:71" x14ac:dyDescent="0.25">
       <c r="X101" s="3">
         <f>VLOOKUP(AA97,$A:$B,2,FALSE)</f>
         <v>4.0999999999999996</v>
@@ -7810,7 +7962,7 @@
       </c>
       <c r="BS101" s="5"/>
     </row>
-    <row r="102" spans="24:71">
+    <row r="102" spans="24:71" x14ac:dyDescent="0.25">
       <c r="X102" s="3"/>
       <c r="Y102" s="4" t="s">
         <v>73</v>
@@ -7830,7 +7982,7 @@
       </c>
       <c r="BS102" s="5"/>
     </row>
-    <row r="103" spans="24:71">
+    <row r="103" spans="24:71" x14ac:dyDescent="0.25">
       <c r="X103" s="3"/>
       <c r="Y103" s="18" t="s">
         <v>63</v>
@@ -7844,7 +7996,7 @@
       <c r="BP103" s="19"/>
       <c r="BS103" s="5"/>
     </row>
-    <row r="104" spans="24:71">
+    <row r="104" spans="24:71" x14ac:dyDescent="0.25">
       <c r="X104" s="3"/>
       <c r="Y104" s="3">
         <f>HLOOKUP(Y103,$F$1:$H$6,6,FALSE)</f>
@@ -7858,16 +8010,16 @@
       </c>
       <c r="BS104" s="5"/>
     </row>
-    <row r="106" spans="24:71">
-      <c r="BO106" s="21" t="s">
+    <row r="106" spans="24:71" x14ac:dyDescent="0.25">
+      <c r="BO106" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="BP106" s="21"/>
-      <c r="BQ106" s="21"/>
-      <c r="BR106" s="21"/>
+      <c r="BP106" s="20"/>
+      <c r="BQ106" s="20"/>
+      <c r="BR106" s="20"/>
       <c r="BS106" s="5"/>
     </row>
-    <row r="107" spans="24:71">
+    <row r="107" spans="24:71" x14ac:dyDescent="0.25">
       <c r="BO107" s="9" t="s">
         <v>68</v>
       </c>
@@ -7884,7 +8036,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="108" spans="24:71">
+    <row r="108" spans="24:71" x14ac:dyDescent="0.25">
       <c r="BN108" s="3">
         <f>VLOOKUP(BO108,$A:$B,2,FALSE)</f>
         <v>3.5</v>
@@ -7906,7 +8058,7 @@
         <v>0.22386537480877111</v>
       </c>
     </row>
-    <row r="109" spans="24:71">
+    <row r="109" spans="24:71" x14ac:dyDescent="0.25">
       <c r="BN109" s="3">
         <f>VLOOKUP(BO109,$A:$B,2,FALSE)</f>
         <v>1.8</v>
@@ -7921,7 +8073,7 @@
       <c r="BR109" s="10"/>
       <c r="BS109" s="5"/>
     </row>
-    <row r="110" spans="24:71">
+    <row r="110" spans="24:71" x14ac:dyDescent="0.25">
       <c r="BN110" s="3"/>
       <c r="BO110" s="9"/>
       <c r="BP110" s="9"/>
@@ -7929,7 +8081,7 @@
       <c r="BR110" s="10"/>
       <c r="BS110" s="5"/>
     </row>
-    <row r="111" spans="24:71">
+    <row r="111" spans="24:71" x14ac:dyDescent="0.25">
       <c r="BN111" s="3"/>
       <c r="BO111" s="9"/>
       <c r="BP111" s="9"/>
@@ -7937,7 +8089,7 @@
       <c r="BR111" s="10"/>
       <c r="BS111" s="5"/>
     </row>
-    <row r="112" spans="24:71">
+    <row r="112" spans="24:71" x14ac:dyDescent="0.25">
       <c r="BN112" s="3">
         <f>VLOOKUP(BQ108,$A:$B,2,FALSE)</f>
         <v>4</v>
@@ -7951,7 +8103,7 @@
       </c>
       <c r="BS112" s="5"/>
     </row>
-    <row r="113" spans="66:71">
+    <row r="113" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN113" s="3"/>
       <c r="BO113" s="4" t="s">
         <v>73</v>
@@ -7962,7 +8114,7 @@
       </c>
       <c r="BS113" s="5"/>
     </row>
-    <row r="114" spans="66:71">
+    <row r="114" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN114" s="3"/>
       <c r="BO114" s="18" t="s">
         <v>63</v>
@@ -7970,7 +8122,7 @@
       <c r="BP114" s="19"/>
       <c r="BS114" s="5"/>
     </row>
-    <row r="115" spans="66:71">
+    <row r="115" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN115" s="3"/>
       <c r="BO115" s="3">
         <f>HLOOKUP(BO114,$F$1:$H$6,6,FALSE)</f>
@@ -7978,16 +8130,16 @@
       </c>
       <c r="BS115" s="5"/>
     </row>
-    <row r="117" spans="66:71">
-      <c r="BO117" s="21" t="s">
+    <row r="117" spans="66:71" x14ac:dyDescent="0.25">
+      <c r="BO117" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="BP117" s="21"/>
-      <c r="BQ117" s="21"/>
-      <c r="BR117" s="21"/>
+      <c r="BP117" s="20"/>
+      <c r="BQ117" s="20"/>
+      <c r="BR117" s="20"/>
       <c r="BS117" s="5"/>
     </row>
-    <row r="118" spans="66:71">
+    <row r="118" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BO118" s="9" t="s">
         <v>68</v>
       </c>
@@ -8004,7 +8156,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="119" spans="66:71">
+    <row r="119" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN119" s="3">
         <f>VLOOKUP(BO119,$A:$B,2,FALSE)</f>
         <v>3.2</v>
@@ -8026,7 +8178,7 @@
         <v>0.18955512572533828</v>
       </c>
     </row>
-    <row r="120" spans="66:71">
+    <row r="120" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN120" s="3">
         <f t="shared" ref="BN120:BN122" si="12">VLOOKUP(BO120,$A:$B,2,FALSE)</f>
         <v>1.8</v>
@@ -8041,7 +8193,7 @@
       <c r="BR120" s="10"/>
       <c r="BS120" s="5"/>
     </row>
-    <row r="121" spans="66:71">
+    <row r="121" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN121" s="3">
         <f t="shared" si="12"/>
         <v>5.2</v>
@@ -8056,7 +8208,7 @@
       <c r="BR121" s="10"/>
       <c r="BS121" s="5"/>
     </row>
-    <row r="122" spans="66:71">
+    <row r="122" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN122" s="3">
         <f t="shared" si="12"/>
         <v>3.5</v>
@@ -8071,7 +8223,7 @@
       <c r="BR122" s="10"/>
       <c r="BS122" s="5"/>
     </row>
-    <row r="123" spans="66:71">
+    <row r="123" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN123" s="3">
         <f>VLOOKUP(BQ119,$A:$B,2,FALSE)</f>
         <v>4.5</v>
@@ -8085,7 +8237,7 @@
       </c>
       <c r="BS123" s="5"/>
     </row>
-    <row r="124" spans="66:71">
+    <row r="124" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN124" s="3"/>
       <c r="BO124" s="4" t="s">
         <v>73</v>
@@ -8096,7 +8248,7 @@
       </c>
       <c r="BS124" s="5"/>
     </row>
-    <row r="125" spans="66:71">
+    <row r="125" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN125" s="3"/>
       <c r="BO125" s="18" t="s">
         <v>63</v>
@@ -8104,7 +8256,7 @@
       <c r="BP125" s="19"/>
       <c r="BS125" s="5"/>
     </row>
-    <row r="126" spans="66:71">
+    <row r="126" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN126" s="3"/>
       <c r="BO126" s="3">
         <f>HLOOKUP(BO125,$F$1:$H$6,6,FALSE)</f>
@@ -8112,16 +8264,16 @@
       </c>
       <c r="BS126" s="5"/>
     </row>
-    <row r="128" spans="66:71">
-      <c r="BO128" s="21" t="s">
+    <row r="128" spans="66:71" x14ac:dyDescent="0.25">
+      <c r="BO128" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="BP128" s="21"/>
-      <c r="BQ128" s="21"/>
-      <c r="BR128" s="21"/>
+      <c r="BP128" s="20"/>
+      <c r="BQ128" s="20"/>
+      <c r="BR128" s="20"/>
       <c r="BS128" s="5"/>
     </row>
-    <row r="129" spans="66:71">
+    <row r="129" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BO129" s="9" t="s">
         <v>68</v>
       </c>
@@ -8138,7 +8290,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="130" spans="66:71">
+    <row r="130" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN130" s="3">
         <f>VLOOKUP(BO130,$A:$B,2,FALSE)</f>
         <v>3.9</v>
@@ -8160,7 +8312,7 @@
         <v>0.22756640344580048</v>
       </c>
     </row>
-    <row r="131" spans="66:71">
+    <row r="131" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN131" s="3">
         <f>VLOOKUP(BO131,$A:$B,2,FALSE)</f>
         <v>4.7</v>
@@ -8175,7 +8327,7 @@
       <c r="BR131" s="10"/>
       <c r="BS131" s="5"/>
     </row>
-    <row r="132" spans="66:71">
+    <row r="132" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN132" s="3"/>
       <c r="BO132" s="9"/>
       <c r="BP132" s="9"/>
@@ -8183,7 +8335,7 @@
       <c r="BR132" s="10"/>
       <c r="BS132" s="5"/>
     </row>
-    <row r="133" spans="66:71">
+    <row r="133" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN133" s="3"/>
       <c r="BO133" s="9"/>
       <c r="BP133" s="9"/>
@@ -8191,7 +8343,7 @@
       <c r="BR133" s="10"/>
       <c r="BS133" s="5"/>
     </row>
-    <row r="134" spans="66:71">
+    <row r="134" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN134" s="3">
         <f>VLOOKUP(BQ130,$A:$B,2,FALSE)</f>
         <v>6</v>
@@ -8205,7 +8357,7 @@
       </c>
       <c r="BS134" s="5"/>
     </row>
-    <row r="135" spans="66:71">
+    <row r="135" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN135" s="3"/>
       <c r="BO135" s="4" t="s">
         <v>73</v>
@@ -8216,7 +8368,7 @@
       </c>
       <c r="BS135" s="5"/>
     </row>
-    <row r="136" spans="66:71">
+    <row r="136" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN136" s="3"/>
       <c r="BO136" s="18" t="s">
         <v>63</v>
@@ -8224,7 +8376,7 @@
       <c r="BP136" s="19"/>
       <c r="BS136" s="5"/>
     </row>
-    <row r="137" spans="66:71">
+    <row r="137" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN137" s="3"/>
       <c r="BO137" s="3">
         <f>HLOOKUP(BO136,$F$1:$H$6,6,FALSE)</f>
@@ -8232,16 +8384,16 @@
       </c>
       <c r="BS137" s="5"/>
     </row>
-    <row r="139" spans="66:71">
-      <c r="BO139" s="21" t="s">
+    <row r="139" spans="66:71" x14ac:dyDescent="0.25">
+      <c r="BO139" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="BP139" s="21"/>
-      <c r="BQ139" s="21"/>
-      <c r="BR139" s="21"/>
+      <c r="BP139" s="20"/>
+      <c r="BQ139" s="20"/>
+      <c r="BR139" s="20"/>
       <c r="BS139" s="5"/>
     </row>
-    <row r="140" spans="66:71">
+    <row r="140" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BO140" s="9" t="s">
         <v>68</v>
       </c>
@@ -8258,7 +8410,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="141" spans="66:71">
+    <row r="141" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN141" s="3">
         <f>VLOOKUP(BO141,$A:$B,2,FALSE)</f>
         <v>5.4</v>
@@ -8280,7 +8432,7 @@
         <v>0.26112759643916905</v>
       </c>
     </row>
-    <row r="142" spans="66:71">
+    <row r="142" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN142" s="3">
         <f>VLOOKUP(BO142,$A:$B,2,FALSE)</f>
         <v>4.4000000000000004</v>
@@ -8295,7 +8447,7 @@
       <c r="BR142" s="10"/>
       <c r="BS142" s="5"/>
     </row>
-    <row r="143" spans="66:71">
+    <row r="143" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN143" s="3">
         <f>VLOOKUP(BO143,$A:$B,2,FALSE)</f>
         <v>4.3</v>
@@ -8310,7 +8462,7 @@
       <c r="BR143" s="10"/>
       <c r="BS143" s="5"/>
     </row>
-    <row r="144" spans="66:71">
+    <row r="144" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN144" s="3"/>
       <c r="BO144" s="9"/>
       <c r="BP144" s="9"/>
@@ -8318,7 +8470,7 @@
       <c r="BR144" s="10"/>
       <c r="BS144" s="5"/>
     </row>
-    <row r="145" spans="66:71">
+    <row r="145" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN145" s="3">
         <f>VLOOKUP(BQ141,$A:$B,2,FALSE)</f>
         <v>4</v>
@@ -8332,7 +8484,7 @@
       </c>
       <c r="BS145" s="5"/>
     </row>
-    <row r="146" spans="66:71">
+    <row r="146" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN146" s="3"/>
       <c r="BO146" s="4" t="s">
         <v>73</v>
@@ -8343,7 +8495,7 @@
       </c>
       <c r="BS146" s="5"/>
     </row>
-    <row r="147" spans="66:71">
+    <row r="147" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN147" s="3"/>
       <c r="BO147" s="18" t="s">
         <v>63</v>
@@ -8351,7 +8503,7 @@
       <c r="BP147" s="19"/>
       <c r="BS147" s="5"/>
     </row>
-    <row r="148" spans="66:71">
+    <row r="148" spans="66:71" x14ac:dyDescent="0.25">
       <c r="BN148" s="3"/>
       <c r="BO148" s="3">
         <f>HLOOKUP(BO147,$F$1:$H$6,6,FALSE)</f>
@@ -8360,20 +8512,108 @@
       <c r="BS148" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="136">
-    <mergeCell ref="CC70:CD70"/>
-    <mergeCell ref="CC48:CD48"/>
-    <mergeCell ref="CC29:CF29"/>
-    <mergeCell ref="CC40:CF40"/>
-    <mergeCell ref="CC51:CF51"/>
-    <mergeCell ref="CC59:CD59"/>
-    <mergeCell ref="CC62:CF62"/>
-    <mergeCell ref="CC3:CF3"/>
-    <mergeCell ref="CC7:CF7"/>
-    <mergeCell ref="CC15:CD15"/>
-    <mergeCell ref="CC18:CF18"/>
-    <mergeCell ref="CC26:CD26"/>
-    <mergeCell ref="CC37:CD37"/>
+  <mergeCells count="138">
+    <mergeCell ref="BV62:BY62"/>
+    <mergeCell ref="BV70:BW70"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="R29:U29"/>
+    <mergeCell ref="R37:S37"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="Y3:AB3"/>
+    <mergeCell ref="Y7:AB7"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y18:AB18"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y29:AB29"/>
+    <mergeCell ref="Y37:Z37"/>
+    <mergeCell ref="Y40:AB40"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="Y81:Z81"/>
+    <mergeCell ref="Y84:AB84"/>
+    <mergeCell ref="Y92:Z92"/>
+    <mergeCell ref="Y95:AB95"/>
+    <mergeCell ref="Y103:Z103"/>
+    <mergeCell ref="Y48:Z48"/>
+    <mergeCell ref="Y51:AB51"/>
+    <mergeCell ref="Y59:Z59"/>
+    <mergeCell ref="Y62:AB62"/>
+    <mergeCell ref="Y70:Z70"/>
+    <mergeCell ref="Y73:AB73"/>
+    <mergeCell ref="AF3:AI3"/>
+    <mergeCell ref="AF7:AI7"/>
+    <mergeCell ref="AF15:AG15"/>
+    <mergeCell ref="AF18:AI18"/>
+    <mergeCell ref="AF26:AG26"/>
+    <mergeCell ref="AF29:AI29"/>
+    <mergeCell ref="AF37:AG37"/>
+    <mergeCell ref="AF40:AI40"/>
+    <mergeCell ref="AF48:AG48"/>
+    <mergeCell ref="AM48:AN48"/>
+    <mergeCell ref="AT3:AW3"/>
+    <mergeCell ref="AT7:AW7"/>
+    <mergeCell ref="AT15:AU15"/>
+    <mergeCell ref="AT18:AW18"/>
+    <mergeCell ref="AT26:AU26"/>
+    <mergeCell ref="AT29:AW29"/>
+    <mergeCell ref="AT37:AU37"/>
+    <mergeCell ref="AT48:AU48"/>
+    <mergeCell ref="AM3:AP3"/>
+    <mergeCell ref="AM7:AP7"/>
+    <mergeCell ref="AM15:AN15"/>
+    <mergeCell ref="AM18:AP18"/>
+    <mergeCell ref="AM26:AN26"/>
+    <mergeCell ref="AM29:AP29"/>
+    <mergeCell ref="AM37:AN37"/>
+    <mergeCell ref="AM40:AP40"/>
+    <mergeCell ref="BA51:BD51"/>
+    <mergeCell ref="BA59:BB59"/>
+    <mergeCell ref="BH3:BK3"/>
+    <mergeCell ref="BH7:BK7"/>
+    <mergeCell ref="BH15:BI15"/>
+    <mergeCell ref="BH18:BK18"/>
+    <mergeCell ref="BH26:BI26"/>
+    <mergeCell ref="BA3:BD3"/>
+    <mergeCell ref="BA7:BD7"/>
+    <mergeCell ref="BA15:BB15"/>
+    <mergeCell ref="BA18:BD18"/>
+    <mergeCell ref="BA26:BB26"/>
+    <mergeCell ref="BA29:BD29"/>
+    <mergeCell ref="BO3:BR3"/>
+    <mergeCell ref="BO7:BR7"/>
+    <mergeCell ref="BO15:BP15"/>
+    <mergeCell ref="BO18:BR18"/>
+    <mergeCell ref="BO26:BP26"/>
+    <mergeCell ref="BO37:BP37"/>
+    <mergeCell ref="BO48:BP48"/>
+    <mergeCell ref="BA37:BB37"/>
+    <mergeCell ref="BA48:BB48"/>
+    <mergeCell ref="BA40:BD40"/>
+    <mergeCell ref="BO103:BP103"/>
+    <mergeCell ref="BO29:BR29"/>
+    <mergeCell ref="BO40:BR40"/>
+    <mergeCell ref="BO51:BR51"/>
+    <mergeCell ref="BO59:BP59"/>
+    <mergeCell ref="BO62:BR62"/>
+    <mergeCell ref="BO70:BP70"/>
+    <mergeCell ref="BH37:BI37"/>
+    <mergeCell ref="BH48:BI48"/>
     <mergeCell ref="BV40:BY40"/>
     <mergeCell ref="BV51:BY51"/>
     <mergeCell ref="BV59:BW59"/>
@@ -8398,105 +8638,19 @@
     <mergeCell ref="BO84:BR84"/>
     <mergeCell ref="BO92:BP92"/>
     <mergeCell ref="BO95:BR95"/>
-    <mergeCell ref="BO103:BP103"/>
-    <mergeCell ref="BO29:BR29"/>
-    <mergeCell ref="BO40:BR40"/>
-    <mergeCell ref="BO51:BR51"/>
-    <mergeCell ref="BO59:BP59"/>
-    <mergeCell ref="BO62:BR62"/>
-    <mergeCell ref="BO70:BP70"/>
-    <mergeCell ref="BH37:BI37"/>
-    <mergeCell ref="BH48:BI48"/>
-    <mergeCell ref="BO3:BR3"/>
-    <mergeCell ref="BO7:BR7"/>
-    <mergeCell ref="BO15:BP15"/>
-    <mergeCell ref="BO18:BR18"/>
-    <mergeCell ref="BO26:BP26"/>
-    <mergeCell ref="BO37:BP37"/>
-    <mergeCell ref="BO48:BP48"/>
-    <mergeCell ref="BA37:BB37"/>
-    <mergeCell ref="BA48:BB48"/>
-    <mergeCell ref="BA40:BD40"/>
-    <mergeCell ref="BA51:BD51"/>
-    <mergeCell ref="BA59:BB59"/>
-    <mergeCell ref="BH3:BK3"/>
-    <mergeCell ref="BH7:BK7"/>
-    <mergeCell ref="BH15:BI15"/>
-    <mergeCell ref="BH18:BK18"/>
-    <mergeCell ref="BH26:BI26"/>
-    <mergeCell ref="BA3:BD3"/>
-    <mergeCell ref="BA7:BD7"/>
-    <mergeCell ref="BA15:BB15"/>
-    <mergeCell ref="BA18:BD18"/>
-    <mergeCell ref="BA26:BB26"/>
-    <mergeCell ref="BA29:BD29"/>
-    <mergeCell ref="AM48:AN48"/>
-    <mergeCell ref="AT3:AW3"/>
-    <mergeCell ref="AT7:AW7"/>
-    <mergeCell ref="AT15:AU15"/>
-    <mergeCell ref="AT18:AW18"/>
-    <mergeCell ref="AT26:AU26"/>
-    <mergeCell ref="AT29:AW29"/>
-    <mergeCell ref="AT37:AU37"/>
-    <mergeCell ref="AT48:AU48"/>
-    <mergeCell ref="AM3:AP3"/>
-    <mergeCell ref="AM7:AP7"/>
-    <mergeCell ref="AM15:AN15"/>
-    <mergeCell ref="AM18:AP18"/>
-    <mergeCell ref="AM26:AN26"/>
-    <mergeCell ref="AM29:AP29"/>
-    <mergeCell ref="AM37:AN37"/>
-    <mergeCell ref="AM40:AP40"/>
-    <mergeCell ref="AF3:AI3"/>
-    <mergeCell ref="AF7:AI7"/>
-    <mergeCell ref="AF15:AG15"/>
-    <mergeCell ref="AF18:AI18"/>
-    <mergeCell ref="AF26:AG26"/>
-    <mergeCell ref="AF29:AI29"/>
-    <mergeCell ref="AF37:AG37"/>
-    <mergeCell ref="AF40:AI40"/>
-    <mergeCell ref="AF48:AG48"/>
-    <mergeCell ref="Y81:Z81"/>
-    <mergeCell ref="Y84:AB84"/>
-    <mergeCell ref="Y92:Z92"/>
-    <mergeCell ref="Y95:AB95"/>
-    <mergeCell ref="Y103:Z103"/>
-    <mergeCell ref="Y48:Z48"/>
-    <mergeCell ref="Y51:AB51"/>
-    <mergeCell ref="Y59:Z59"/>
-    <mergeCell ref="Y62:AB62"/>
-    <mergeCell ref="Y70:Z70"/>
-    <mergeCell ref="Y73:AB73"/>
-    <mergeCell ref="Y3:AB3"/>
-    <mergeCell ref="Y7:AB7"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="Y18:AB18"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y29:AB29"/>
-    <mergeCell ref="Y37:Z37"/>
-    <mergeCell ref="Y40:AB40"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="K81:L81"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="R29:U29"/>
-    <mergeCell ref="R37:S37"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="K62:N62"/>
-    <mergeCell ref="K70:L70"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="CC70:CD70"/>
+    <mergeCell ref="CC48:CD48"/>
+    <mergeCell ref="CC29:CF29"/>
+    <mergeCell ref="CC40:CF40"/>
+    <mergeCell ref="CC51:CF51"/>
+    <mergeCell ref="CC59:CD59"/>
+    <mergeCell ref="CC62:CF62"/>
+    <mergeCell ref="CC3:CF3"/>
+    <mergeCell ref="CC7:CF7"/>
+    <mergeCell ref="CC15:CD15"/>
+    <mergeCell ref="CC18:CF18"/>
+    <mergeCell ref="CC26:CD26"/>
+    <mergeCell ref="CC37:CD37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8504,19 +8658,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8524,7 +8678,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8532,7 +8686,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8540,7 +8694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -8548,7 +8702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -8556,7 +8710,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8564,7 +8718,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -8572,7 +8726,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -8580,7 +8734,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -8588,7 +8742,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -8596,7 +8750,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -8604,7 +8758,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -8612,7 +8766,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -8620,7 +8774,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -8628,7 +8782,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -8636,7 +8790,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -8644,7 +8798,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -8652,7 +8806,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -8660,7 +8814,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -8668,7 +8822,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -8676,7 +8830,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -8684,7 +8838,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -8692,7 +8846,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -8700,7 +8854,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -8708,7 +8862,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -8716,7 +8870,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -8724,7 +8878,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -8732,7 +8886,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -8740,7 +8894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -8748,7 +8902,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -8756,7 +8910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -8764,7 +8918,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -8772,7 +8926,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -8780,7 +8934,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -8788,7 +8942,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -8796,7 +8950,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -8804,7 +8958,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -8812,7 +8966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -8820,7 +8974,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -8828,7 +8982,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -8836,7 +8990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -8844,7 +8998,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -8852,7 +9006,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -8860,7 +9014,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -8868,7 +9022,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -8876,7 +9030,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -8884,7 +9038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -8892,7 +9046,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -8900,7 +9054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -8908,7 +9062,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -8916,7 +9070,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -8924,7 +9078,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -8932,7 +9086,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -8940,7 +9094,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -8948,7 +9102,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -8956,7 +9110,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -8964,7 +9118,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -8972,7 +9126,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -8980,7 +9134,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -8988,7 +9142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -8996,7 +9150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -9004,7 +9158,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -9012,7 +9166,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -9027,12 +9181,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>